<commit_message>
terrain boss2, changed glyph a bit
</commit_message>
<xml_diff>
--- a/dev/Items.xlsx
+++ b/dev/Items.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="Glyph" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="742">
   <si>
     <t>名称</t>
   </si>
@@ -2144,39 +2144,9 @@
     <t>等级</t>
   </si>
   <si>
-    <t>使用后恢复20%的法力值。</t>
-  </si>
-  <si>
-    <t>使用后恢复40%的法力值。</t>
-  </si>
-  <si>
-    <t>使用后恢复10%的法力值。</t>
-  </si>
-  <si>
-    <t>使用后恢复30%的法力值。</t>
-  </si>
-  <si>
     <t>“坚毅”</t>
   </si>
   <si>
-    <t>每秒恢复5点生命值，使用后恢复10%的生命值。</t>
-  </si>
-  <si>
-    <t>每秒恢复10点生命值，使用后恢复20%的生命值。</t>
-  </si>
-  <si>
-    <t>每秒恢复15点生命值，使用后恢复30%的生命值。</t>
-  </si>
-  <si>
-    <t>每秒恢复20点生命值，使用后恢复40%的生命值。</t>
-  </si>
-  <si>
-    <t>使用后恢复50%的法力值。并且在接下来的10秒内，每秒恢复5%的法力值。</t>
-  </si>
-  <si>
-    <t>每秒恢复1%的生命值，至少恢复30点，使用后恢复50%的生命值。</t>
-  </si>
-  <si>
     <t>“活力”</t>
   </si>
   <si>
@@ -2228,9 +2198,6 @@
     <t>+20力量，攻击时有一定几率对附近200码范围内的一个敌人造成等同伤害，如果没有额外目标，那么对当前目标造成50%额外伤害。</t>
   </si>
   <si>
-    <t>+50攻击强度，开启后，造成的所有伤害提高30%，持续15秒。</t>
-  </si>
-  <si>
     <t>“智者”</t>
   </si>
   <si>
@@ -2271,6 +2238,24 @@
   </si>
   <si>
     <t>“强袭”</t>
+  </si>
+  <si>
+    <t>回血回蓝</t>
+  </si>
+  <si>
+    <t>+10攻击强度，+15法术强度</t>
+  </si>
+  <si>
+    <t>+20攻击强度，+30法术强度</t>
+  </si>
+  <si>
+    <t>+30攻击强度，+45法术强度</t>
+  </si>
+  <si>
+    <t>+40攻击强度，+60法术强度</t>
+  </si>
+  <si>
+    <t>+50攻击强度，+75法术强度，开启后，造成的所有伤害提高30%，持续15秒。</t>
   </si>
 </sst>
 </file>
@@ -2687,13 +2672,13 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4921,16 +4906,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="77" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" style="72" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="114.140625" style="61" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" style="67" bestFit="1" customWidth="1"/>
@@ -4939,7 +4924,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="62" t="s">
-        <v>745</v>
+        <v>734</v>
       </c>
       <c r="B1" s="70" t="s">
         <v>703</v>
@@ -4953,13 +4938,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="66" t="s">
-        <v>726</v>
+        <v>716</v>
       </c>
       <c r="B2" s="69">
         <v>1</v>
       </c>
-      <c r="C2" s="77" t="s">
-        <v>727</v>
+      <c r="C2" s="76" t="s">
+        <v>717</v>
       </c>
       <c r="D2" s="73"/>
     </row>
@@ -4968,8 +4953,8 @@
       <c r="B3" s="69">
         <v>2</v>
       </c>
-      <c r="C3" s="77" t="s">
-        <v>728</v>
+      <c r="C3" s="76" t="s">
+        <v>718</v>
       </c>
       <c r="D3" s="73"/>
     </row>
@@ -4978,8 +4963,8 @@
       <c r="B4" s="69">
         <v>3</v>
       </c>
-      <c r="C4" s="77" t="s">
-        <v>729</v>
+      <c r="C4" s="76" t="s">
+        <v>719</v>
       </c>
       <c r="D4" s="73"/>
     </row>
@@ -4988,8 +4973,8 @@
       <c r="B5" s="69">
         <v>4</v>
       </c>
-      <c r="C5" s="77" t="s">
-        <v>730</v>
+      <c r="C5" s="76" t="s">
+        <v>720</v>
       </c>
       <c r="D5" s="73"/>
     </row>
@@ -4998,20 +4983,20 @@
       <c r="B6" s="69">
         <v>5</v>
       </c>
-      <c r="C6" s="77" t="s">
-        <v>731</v>
+      <c r="C6" s="76" t="s">
+        <v>721</v>
       </c>
       <c r="D6" s="73"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="66" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
       <c r="B7" s="68">
         <v>1</v>
       </c>
-      <c r="C7" s="77" t="s">
-        <v>740</v>
+      <c r="C7" s="76" t="s">
+        <v>729</v>
       </c>
       <c r="D7" s="73"/>
     </row>
@@ -5020,8 +5005,8 @@
       <c r="B8" s="68">
         <v>2</v>
       </c>
-      <c r="C8" s="77" t="s">
-        <v>741</v>
+      <c r="C8" s="76" t="s">
+        <v>730</v>
       </c>
       <c r="D8" s="73"/>
     </row>
@@ -5030,8 +5015,8 @@
       <c r="B9" s="68">
         <v>3</v>
       </c>
-      <c r="C9" s="77" t="s">
-        <v>742</v>
+      <c r="C9" s="76" t="s">
+        <v>731</v>
       </c>
       <c r="D9" s="73"/>
     </row>
@@ -5040,8 +5025,8 @@
       <c r="B10" s="68">
         <v>4</v>
       </c>
-      <c r="C10" s="77" t="s">
-        <v>743</v>
+      <c r="C10" s="76" t="s">
+        <v>732</v>
       </c>
       <c r="D10" s="73"/>
     </row>
@@ -5050,20 +5035,20 @@
       <c r="B11" s="68">
         <v>5</v>
       </c>
-      <c r="C11" s="77" t="s">
-        <v>744</v>
+      <c r="C11" s="76" t="s">
+        <v>733</v>
       </c>
       <c r="D11" s="73"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="66" t="s">
-        <v>733</v>
+        <v>722</v>
       </c>
       <c r="B12" s="69">
         <v>1</v>
       </c>
-      <c r="C12" s="77" t="s">
-        <v>734</v>
+      <c r="C12" s="76" t="s">
+        <v>723</v>
       </c>
       <c r="D12" s="73"/>
     </row>
@@ -5072,8 +5057,8 @@
       <c r="B13" s="69">
         <v>2</v>
       </c>
-      <c r="C13" s="77" t="s">
-        <v>735</v>
+      <c r="C13" s="76" t="s">
+        <v>724</v>
       </c>
       <c r="D13" s="73"/>
     </row>
@@ -5082,8 +5067,8 @@
       <c r="B14" s="69">
         <v>3</v>
       </c>
-      <c r="C14" s="77" t="s">
-        <v>736</v>
+      <c r="C14" s="76" t="s">
+        <v>725</v>
       </c>
       <c r="D14" s="73"/>
     </row>
@@ -5092,8 +5077,8 @@
       <c r="B15" s="69">
         <v>4</v>
       </c>
-      <c r="C15" s="77" t="s">
-        <v>737</v>
+      <c r="C15" s="76" t="s">
+        <v>726</v>
       </c>
       <c r="D15" s="73"/>
     </row>
@@ -5102,8 +5087,8 @@
       <c r="B16" s="69">
         <v>5</v>
       </c>
-      <c r="C16" s="77" t="s">
-        <v>739</v>
+      <c r="C16" s="76" t="s">
+        <v>728</v>
       </c>
       <c r="D16" s="73"/>
     </row>
@@ -5114,8 +5099,8 @@
       <c r="B17" s="68">
         <v>1</v>
       </c>
-      <c r="C17" s="77" t="s">
-        <v>721</v>
+      <c r="C17" s="76" t="s">
+        <v>711</v>
       </c>
       <c r="D17" s="73"/>
     </row>
@@ -5124,8 +5109,8 @@
       <c r="B18" s="68">
         <v>2</v>
       </c>
-      <c r="C18" s="77" t="s">
-        <v>722</v>
+      <c r="C18" s="76" t="s">
+        <v>712</v>
       </c>
       <c r="D18" s="73"/>
     </row>
@@ -5134,8 +5119,8 @@
       <c r="B19" s="68">
         <v>3</v>
       </c>
-      <c r="C19" s="77" t="s">
-        <v>723</v>
+      <c r="C19" s="76" t="s">
+        <v>713</v>
       </c>
       <c r="D19" s="73"/>
     </row>
@@ -5144,8 +5129,8 @@
       <c r="B20" s="68">
         <v>4</v>
       </c>
-      <c r="C20" s="77" t="s">
-        <v>724</v>
+      <c r="C20" s="76" t="s">
+        <v>714</v>
       </c>
       <c r="D20" s="73"/>
     </row>
@@ -5154,8 +5139,8 @@
       <c r="B21" s="68">
         <v>5</v>
       </c>
-      <c r="C21" s="77" t="s">
-        <v>725</v>
+      <c r="C21" s="76" t="s">
+        <v>715</v>
       </c>
       <c r="D21" s="73">
         <v>60</v>
@@ -5163,13 +5148,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="66" t="s">
-        <v>746</v>
+        <v>735</v>
       </c>
       <c r="B22" s="68">
         <v>1</v>
       </c>
-      <c r="C22" s="77" t="s">
-        <v>206</v>
+      <c r="C22" s="76" t="s">
+        <v>737</v>
       </c>
       <c r="D22" s="73"/>
     </row>
@@ -5178,8 +5163,8 @@
       <c r="B23" s="68">
         <v>2</v>
       </c>
-      <c r="C23" s="77" t="s">
-        <v>639</v>
+      <c r="C23" s="76" t="s">
+        <v>738</v>
       </c>
       <c r="D23" s="73"/>
     </row>
@@ -5188,8 +5173,8 @@
       <c r="B24" s="68">
         <v>3</v>
       </c>
-      <c r="C24" s="77" t="s">
-        <v>642</v>
+      <c r="C24" s="76" t="s">
+        <v>739</v>
       </c>
       <c r="D24" s="73"/>
     </row>
@@ -5198,8 +5183,8 @@
       <c r="B25" s="68">
         <v>4</v>
       </c>
-      <c r="C25" s="77" t="s">
-        <v>654</v>
+      <c r="C25" s="76" t="s">
+        <v>740</v>
       </c>
       <c r="D25" s="73"/>
     </row>
@@ -5208,8 +5193,8 @@
       <c r="B26" s="68">
         <v>5</v>
       </c>
-      <c r="C26" s="77" t="s">
-        <v>732</v>
+      <c r="C26" s="76" t="s">
+        <v>741</v>
       </c>
       <c r="D26" s="73">
         <v>60</v>
@@ -5217,13 +5202,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="75" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="B27" s="71">
         <v>1</v>
       </c>
-      <c r="C27" s="77" t="s">
-        <v>716</v>
+      <c r="C27" s="76" t="s">
+        <v>706</v>
       </c>
       <c r="D27" s="73">
         <v>60</v>
@@ -5234,8 +5219,8 @@
       <c r="B28" s="71">
         <v>2</v>
       </c>
-      <c r="C28" s="77" t="s">
-        <v>717</v>
+      <c r="C28" s="76" t="s">
+        <v>707</v>
       </c>
       <c r="D28" s="73">
         <v>60</v>
@@ -5246,8 +5231,8 @@
       <c r="B29" s="71">
         <v>3</v>
       </c>
-      <c r="C29" s="77" t="s">
-        <v>718</v>
+      <c r="C29" s="76" t="s">
+        <v>708</v>
       </c>
       <c r="D29" s="73">
         <v>60</v>
@@ -5258,8 +5243,8 @@
       <c r="B30" s="71">
         <v>4</v>
       </c>
-      <c r="C30" s="77" t="s">
-        <v>719</v>
+      <c r="C30" s="76" t="s">
+        <v>709</v>
       </c>
       <c r="D30" s="73">
         <v>60</v>
@@ -5270,8 +5255,8 @@
       <c r="B31" s="71">
         <v>5</v>
       </c>
-      <c r="C31" s="77" t="s">
-        <v>720</v>
+      <c r="C31" s="76" t="s">
+        <v>710</v>
       </c>
       <c r="D31" s="73">
         <v>60</v>
@@ -5279,65 +5264,47 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="66" t="s">
-        <v>715</v>
+        <v>705</v>
       </c>
       <c r="B32" s="69">
         <v>1</v>
       </c>
       <c r="C32" s="65" t="s">
-        <v>709</v>
-      </c>
-      <c r="D32" s="73">
-        <v>60</v>
-      </c>
+        <v>736</v>
+      </c>
+      <c r="D32" s="73"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="75"/>
       <c r="B33" s="69">
         <v>2</v>
       </c>
-      <c r="C33" s="65" t="s">
-        <v>710</v>
-      </c>
-      <c r="D33" s="73">
-        <v>60</v>
-      </c>
+      <c r="C33" s="65"/>
+      <c r="D33" s="73"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="75"/>
       <c r="B34" s="69">
         <v>3</v>
       </c>
-      <c r="C34" s="65" t="s">
-        <v>711</v>
-      </c>
-      <c r="D34" s="73">
-        <v>60</v>
-      </c>
+      <c r="C34" s="65"/>
+      <c r="D34" s="73"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="75"/>
       <c r="B35" s="69">
         <v>4</v>
       </c>
-      <c r="C35" s="65" t="s">
-        <v>712</v>
-      </c>
-      <c r="D35" s="73">
-        <v>60</v>
-      </c>
+      <c r="C35" s="65"/>
+      <c r="D35" s="73"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="75"/>
       <c r="B36" s="69">
         <v>5</v>
       </c>
-      <c r="C36" s="65" t="s">
-        <v>714</v>
-      </c>
-      <c r="D36" s="73">
-        <v>60</v>
-      </c>
+      <c r="C36" s="65"/>
+      <c r="D36" s="73"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="66" t="s">
@@ -5347,59 +5314,41 @@
         <v>1</v>
       </c>
       <c r="C37" s="65" t="s">
-        <v>706</v>
-      </c>
-      <c r="D37" s="73">
-        <v>60</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D37" s="73"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="66"/>
       <c r="B38" s="68">
         <v>2</v>
       </c>
-      <c r="C38" s="65" t="s">
-        <v>704</v>
-      </c>
-      <c r="D38" s="73">
-        <v>60</v>
-      </c>
+      <c r="C38" s="65"/>
+      <c r="D38" s="73"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="66"/>
       <c r="B39" s="68">
         <v>3</v>
       </c>
-      <c r="C39" s="65" t="s">
-        <v>707</v>
-      </c>
-      <c r="D39" s="73">
-        <v>60</v>
-      </c>
+      <c r="C39" s="65"/>
+      <c r="D39" s="73"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="66"/>
       <c r="B40" s="68">
         <v>4</v>
       </c>
-      <c r="C40" s="65" t="s">
-        <v>705</v>
-      </c>
-      <c r="D40" s="73">
-        <v>60</v>
-      </c>
+      <c r="C40" s="65"/>
+      <c r="D40" s="73"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="66"/>
       <c r="B41" s="68">
         <v>5</v>
       </c>
-      <c r="C41" s="65" t="s">
-        <v>713</v>
-      </c>
-      <c r="D41" s="73">
-        <v>60</v>
-      </c>
+      <c r="C41" s="65"/>
+      <c r="D41" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5425,18 +5374,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="54"/>
@@ -6697,7 +6646,7 @@
       <c r="J2" s="57"/>
       <c r="K2" s="58">
         <f t="shared" ref="K2:K97" ca="1" si="2">RAND() * 100</f>
-        <v>49.445172602033061</v>
+        <v>89.515164256506836</v>
       </c>
       <c r="L2" s="57" t="str">
         <f ca="1">IF(K2&lt;=C2, IF(K2&lt;H2,$A$2,IF(K2&lt;H3,$A$3, IF(K2&lt;H4,$A$4, IF(K2&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6749,7 +6698,7 @@
       <c r="J3" s="57"/>
       <c r="K3" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>90.360115537417741</v>
+        <v>73.665107384882106</v>
       </c>
       <c r="L3" s="57" t="str">
         <f ca="1">IF(K3&lt;=C3, IF(K3&lt;H2,$A$2,IF(K3&lt;H3,$A$3, IF(K3&lt;H4,$A$4, IF(K3&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6801,7 +6750,7 @@
       <c r="J4" s="57"/>
       <c r="K4" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>36.287699483899971</v>
+        <v>45.510502644926312</v>
       </c>
       <c r="L4" s="57" t="str">
         <f ca="1">IF(K4&lt;=C4, IF(K4&lt;H2,$A$2,IF(K4&lt;H3,$A$3, IF(K4&lt;H4,$A$4, IF(K4&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6853,7 +6802,7 @@
       <c r="J5" s="57"/>
       <c r="K5" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7644979333912967</v>
+        <v>65.122311518877751</v>
       </c>
       <c r="L5" s="57" t="str">
         <f ca="1">IF(K5&lt;=C5, IF(K5&lt;H2,$A$2,IF(K5&lt;H3,$A$3, IF(K5&lt;H4,$A$4, IF(K5&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6902,7 +6851,7 @@
       </c>
       <c r="K6" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>91.310383571274201</v>
+        <v>89.708680373627658</v>
       </c>
       <c r="L6" s="57" t="str">
         <f ca="1">IF(K6&lt;=C6, IF(K6&lt;H6,$A$2,IF(K6&lt;H7,$A$3, IF(K6&lt;H8,$A$4, IF(K6&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -6943,7 +6892,7 @@
       </c>
       <c r="K7" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>20.421077915275454</v>
+        <v>62.801510345181512</v>
       </c>
       <c r="L7" s="57" t="str">
         <f ca="1">IF(K7&lt;=C7, IF(K7&lt;H6,$A$2,IF(K7&lt;H7,$A$3, IF(K7&lt;H8,$A$4, IF(K7&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -6984,7 +6933,7 @@
       </c>
       <c r="K8" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>15.435654907396511</v>
+        <v>96.250267964913618</v>
       </c>
       <c r="L8" s="57" t="str">
         <f ca="1">IF(K8&lt;=C8, IF(K8&lt;H6,$A$2,IF(K8&lt;H7,$A$3, IF(K8&lt;H8,$A$4, IF(K8&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -7025,7 +6974,7 @@
       </c>
       <c r="K9" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>34.64793090851542</v>
+        <v>38.367163571491744</v>
       </c>
       <c r="L9" s="57" t="str">
         <f ca="1">IF(K9&lt;=C9, IF(K9&lt;H6,$A$2,IF(K9&lt;H7,$A$3, IF(K9&lt;H8,$A$4, IF(K9&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -7068,7 +7017,7 @@
       <c r="J10" s="57"/>
       <c r="K10" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>80.38330168632757</v>
+        <v>13.325590370755325</v>
       </c>
       <c r="L10" s="57" t="str">
         <f ca="1">IF(K10&lt;=C10, IF(K10&lt;H10,$A$2,IF(K10&lt;H11,$A$3, IF(K10&lt;H12,$A$4, IF(K10&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -7119,7 +7068,7 @@
       <c r="J11" s="57"/>
       <c r="K11" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>75.871723109666661</v>
+        <v>73.912497302239586</v>
       </c>
       <c r="L11" s="57" t="str">
         <f ca="1">IF(K11&lt;=C11, IF(K11&lt;H10,$A$2,IF(K11&lt;H11,$A$3, IF(K11&lt;H12,$A$4, IF(K11&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -7170,7 +7119,7 @@
       <c r="J12" s="57"/>
       <c r="K12" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>93.011479563806887</v>
+        <v>94.267917965426591</v>
       </c>
       <c r="L12" s="57" t="str">
         <f ca="1">IF(K12&lt;=C12, IF(K12&lt;H10,$A$2,IF(K12&lt;H11,$A$3, IF(K12&lt;H12,$A$4, IF(K12&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -7221,11 +7170,11 @@
       <c r="J13" s="57"/>
       <c r="K13" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>72.987370570651322</v>
+        <v>4.6994938435253708</v>
       </c>
       <c r="L13" s="57" t="str">
         <f ca="1">IF(K13&lt;=C13, IF(K13&lt;H10,$A$2,IF(K13&lt;H11,$A$3, IF(K13&lt;H12,$A$4, IF(K13&lt;H13,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_COMMON</v>
       </c>
       <c r="M13" s="57"/>
       <c r="N13" s="57"/>
@@ -7270,11 +7219,11 @@
       </c>
       <c r="K14" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>5.6333044740706768</v>
+        <v>65.991431308583259</v>
       </c>
       <c r="L14" s="57" t="str">
         <f ca="1">IF(K14&lt;=C14, IF(K14&lt;H14,$A$2,IF(K14&lt;H15,$A$3, IF(K14&lt;H16,$A$4, IF(K14&lt;H17,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_COMMON</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -7311,7 +7260,7 @@
       </c>
       <c r="K15" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>95.861794789542714</v>
+        <v>54.4632550179155</v>
       </c>
       <c r="L15" s="57" t="str">
         <f ca="1">IF(K15&lt;=C15, IF(K15&lt;H14,$A$2,IF(K15&lt;H15,$A$3, IF(K15&lt;H16,$A$4, IF(K15&lt;H17,$A$5, "NONE")))), "NONE")</f>
@@ -7352,7 +7301,7 @@
       </c>
       <c r="K16" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>31.75096179464585</v>
+        <v>71.754273508158818</v>
       </c>
       <c r="L16" s="57" t="str">
         <f ca="1">IF(K16&lt;=C16, IF(K16&lt;H14,$A$2,IF(K16&lt;H15,$A$3, IF(K16&lt;H16,$A$4, IF(K16&lt;H17,$A$5, "NONE")))), "NONE")</f>
@@ -7393,11 +7342,11 @@
       </c>
       <c r="K17" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>3.1474308038464294</v>
+        <v>70.743470366639315</v>
       </c>
       <c r="L17" s="57" t="str">
         <f ca="1">IF(K17&lt;=C17, IF(K17&lt;H14,$A$2,IF(K17&lt;H15,$A$3, IF(K17&lt;H16,$A$4, IF(K17&lt;H17,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -7436,7 +7385,7 @@
       <c r="J18" s="57"/>
       <c r="K18" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>51.955843125638438</v>
+        <v>38.872549778224339</v>
       </c>
       <c r="L18" s="57" t="str">
         <f ca="1">IF(K18&lt;=C18, IF(K18&lt;H18,$A$2,IF(K18&lt;H19,$A$3, IF(K18&lt;H20,$A$4, IF(K18&lt;H21,$A$5, "NONE")))), "NONE")</f>
@@ -7487,11 +7436,11 @@
       <c r="J19" s="57"/>
       <c r="K19" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>4.9423030545782787</v>
+        <v>81.308817359768454</v>
       </c>
       <c r="L19" s="57" t="str">
         <f ca="1">IF(K19&lt;=C19, IF(K19&lt;H18,$A$2,IF(K19&lt;H19,$A$3, IF(K19&lt;H20,$A$4, IF(K19&lt;H21,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
       <c r="M19" s="57"/>
       <c r="N19" s="57"/>
@@ -7538,7 +7487,7 @@
       <c r="J20" s="57"/>
       <c r="K20" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>41.913953678066918</v>
+        <v>30.323072115809889</v>
       </c>
       <c r="L20" s="57" t="str">
         <f ca="1">IF(K20&lt;=C20, IF(K20&lt;H18,$A$2,IF(K20&lt;H19,$A$3, IF(K20&lt;H20,$A$4, IF(K20&lt;H21,$A$5, "NONE")))), "NONE")</f>
@@ -7589,7 +7538,7 @@
       <c r="J21" s="57"/>
       <c r="K21" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>71.143427476819909</v>
+        <v>91.246924605969681</v>
       </c>
       <c r="L21" s="57" t="str">
         <f ca="1">IF(K21&lt;=C21, IF(K21&lt;H18,$A$2,IF(K21&lt;H19,$A$3, IF(K21&lt;H20,$A$4, IF(K21&lt;H21,$A$5, "NONE")))), "NONE")</f>
@@ -7638,7 +7587,7 @@
       </c>
       <c r="K22" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>93.827264185927788</v>
+        <v>64.80661148505267</v>
       </c>
       <c r="L22" s="57" t="str">
         <f ca="1">IF(K22&lt;=C22, IF(K22&lt;H22,$A$2,IF(K22&lt;H23,$A$3, IF(K22&lt;H24,$A$4, IF(K22&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7679,7 +7628,7 @@
       </c>
       <c r="K23" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>80.414363551557884</v>
+        <v>43.426507116641901</v>
       </c>
       <c r="L23" s="57" t="str">
         <f ca="1">IF(K23&lt;=C23, IF(K23&lt;H22,$A$2,IF(K23&lt;H23,$A$3, IF(K23&lt;H24,$A$4, IF(K23&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7720,7 +7669,7 @@
       </c>
       <c r="K24" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>48.456790747359271</v>
+        <v>70.090676100752276</v>
       </c>
       <c r="L24" s="57" t="str">
         <f ca="1">IF(K24&lt;=C24, IF(K24&lt;H22,$A$2,IF(K24&lt;H23,$A$3, IF(K24&lt;H24,$A$4, IF(K24&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7761,7 +7710,7 @@
       </c>
       <c r="K25" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>72.435995361917648</v>
+        <v>29.718435307948752</v>
       </c>
       <c r="L25" s="57" t="str">
         <f ca="1">IF(K25&lt;=C25, IF(K25&lt;H22,$A$2,IF(K25&lt;H23,$A$3, IF(K25&lt;H24,$A$4, IF(K25&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7804,7 +7753,7 @@
       <c r="J26" s="57"/>
       <c r="K26" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>78.956433977076728</v>
+        <v>20.968276468607584</v>
       </c>
       <c r="L26" s="57" t="str">
         <f ca="1">IF(K26&lt;=C26, IF(K26&lt;H26,$A$2,IF(K26&lt;H27,$A$3, IF(K26&lt;H28,$A$4, IF(K26&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7855,7 +7804,7 @@
       <c r="J27" s="57"/>
       <c r="K27" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8050375064611863</v>
+        <v>5.7834478898587616</v>
       </c>
       <c r="L27" s="57" t="str">
         <f ca="1">IF(K27&lt;=C27, IF(K27&lt;H26,$A$2,IF(K27&lt;H27,$A$3, IF(K27&lt;H28,$A$4, IF(K27&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7906,7 +7855,7 @@
       <c r="J28" s="57"/>
       <c r="K28" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>60.082740269342494</v>
+        <v>24.139328023826799</v>
       </c>
       <c r="L28" s="57" t="str">
         <f ca="1">IF(K28&lt;=C28, IF(K28&lt;H26,$A$2,IF(K28&lt;H27,$A$3, IF(K28&lt;H28,$A$4, IF(K28&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7957,7 +7906,7 @@
       <c r="J29" s="57"/>
       <c r="K29" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>28.22307038888766</v>
+        <v>48.492086000916231</v>
       </c>
       <c r="L29" s="57" t="str">
         <f ca="1">IF(K29&lt;=C29, IF(K29&lt;H26,$A$2,IF(K29&lt;H27,$A$3, IF(K29&lt;H28,$A$4, IF(K29&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -8006,7 +7955,7 @@
       </c>
       <c r="K30" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>86.03409631431019</v>
+        <v>92.219008758623062</v>
       </c>
       <c r="L30" s="57" t="str">
         <f ca="1">IF(K30&lt;=C30, IF(K30&lt;H30,$A$2,IF(K30&lt;H31,$A$3, IF(K30&lt;H32,$A$4, IF(K30&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -8047,7 +7996,7 @@
       </c>
       <c r="K31" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>76.47890535906366</v>
+        <v>38.886563751032476</v>
       </c>
       <c r="L31" s="57" t="str">
         <f ca="1">IF(K31&lt;=C31, IF(K31&lt;H30,$A$2,IF(K31&lt;H31,$A$3, IF(K31&lt;H32,$A$4, IF(K31&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -8088,11 +8037,11 @@
       </c>
       <c r="K32" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>6.1007904649358906</v>
+        <v>20.991973983956068</v>
       </c>
       <c r="L32" s="57" t="str">
         <f ca="1">IF(K32&lt;=C32, IF(K32&lt;H30,$A$2,IF(K32&lt;H31,$A$3, IF(K32&lt;H32,$A$4, IF(K32&lt;H33,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -8129,7 +8078,7 @@
       </c>
       <c r="K33" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>89.136096138838724</v>
+        <v>79.91814958989481</v>
       </c>
       <c r="L33" s="57" t="str">
         <f ca="1">IF(K33&lt;=C33, IF(K33&lt;H30,$A$2,IF(K33&lt;H31,$A$3, IF(K33&lt;H32,$A$4, IF(K33&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -8172,7 +8121,7 @@
       <c r="J34" s="57"/>
       <c r="K34" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>50.595911752907483</v>
+        <v>82.703556829610875</v>
       </c>
       <c r="L34" s="57" t="str">
         <f ca="1">IF(K34&lt;=C34, IF(K34&lt;H34,$A$2,IF(K34&lt;H35,$A$3, IF(K34&lt;H36,$A$4, IF(K34&lt;H37,$A$5, "NONE")))), "NONE")</f>
@@ -8223,7 +8172,7 @@
       <c r="J35" s="57"/>
       <c r="K35" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>19.878248501545627</v>
+        <v>38.556461401103157</v>
       </c>
       <c r="L35" s="57" t="str">
         <f ca="1">IF(K35&lt;=C35, IF(K35&lt;H34,$A$2,IF(K35&lt;H35,$A$3, IF(K35&lt;H36,$A$4, IF(K35&lt;H37,$A$5, "NONE")))), "NONE")</f>
@@ -8274,11 +8223,11 @@
       <c r="J36" s="57"/>
       <c r="K36" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>67.038340280033609</v>
+        <v>3.2958917240260011</v>
       </c>
       <c r="L36" s="57" t="str">
         <f ca="1">IF(K36&lt;=C36, IF(K36&lt;H34,$A$2,IF(K36&lt;H35,$A$3, IF(K36&lt;H36,$A$4, IF(K36&lt;H37,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
       <c r="M36" s="57"/>
       <c r="N36" s="57"/>
@@ -8325,7 +8274,7 @@
       <c r="J37" s="57"/>
       <c r="K37" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>97.906101652739849</v>
+        <v>65.337251964664503</v>
       </c>
       <c r="L37" s="57" t="str">
         <f ca="1">IF(K37&lt;=C37, IF(K37&lt;H34,$A$2,IF(K37&lt;H35,$A$3, IF(K37&lt;H36,$A$4, IF(K37&lt;H37,$A$5, "NONE")))), "NONE")</f>
@@ -8374,11 +8323,11 @@
       </c>
       <c r="K38" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>16.279527214460654</v>
+        <v>77.183058332104366</v>
       </c>
       <c r="L38" s="57" t="str">
         <f ca="1">IF(K38&lt;=C38, IF(K38&lt;H38,$A$2,IF(K38&lt;H39,$A$3, IF(K38&lt;H40,$A$4, IF(K38&lt;H41,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_COMMON</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
@@ -8415,11 +8364,11 @@
       </c>
       <c r="K39" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>98.821354272389314</v>
+        <v>2.5671741770952217</v>
       </c>
       <c r="L39" s="57" t="str">
         <f ca="1">IF(K39&lt;=C39, IF(K39&lt;H38,$A$2,IF(K39&lt;H39,$A$3, IF(K39&lt;H40,$A$4, IF(K39&lt;H41,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -8456,7 +8405,7 @@
       </c>
       <c r="K40" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>93.159873145700431</v>
+        <v>90.032962257352452</v>
       </c>
       <c r="L40" s="57" t="str">
         <f ca="1">IF(K40&lt;=C40, IF(K40&lt;H38,$A$2,IF(K40&lt;H39,$A$3, IF(K40&lt;H40,$A$4, IF(K40&lt;H41,$A$5, "NONE")))), "NONE")</f>
@@ -8497,7 +8446,7 @@
       </c>
       <c r="K41" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>58.75534126556402</v>
+        <v>88.822534146551874</v>
       </c>
       <c r="L41" s="57" t="str">
         <f ca="1">IF(K41&lt;=C41, IF(K41&lt;H38,$A$2,IF(K41&lt;H39,$A$3, IF(K41&lt;H40,$A$4, IF(K41&lt;H41,$A$5, "NONE")))), "NONE")</f>
@@ -8540,7 +8489,7 @@
       <c r="J42" s="57"/>
       <c r="K42" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>41.422350277063522</v>
+        <v>42.300581671091699</v>
       </c>
       <c r="L42" s="57" t="str">
         <f ca="1">IF(K42&lt;=C42, IF(K42&lt;H42,$A$2,IF(K42&lt;H43,$A$3, IF(K42&lt;H44,$A$4, IF(K42&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8591,7 +8540,7 @@
       <c r="J43" s="57"/>
       <c r="K43" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>65.228595203319756</v>
+        <v>52.482379688702906</v>
       </c>
       <c r="L43" s="57" t="str">
         <f ca="1">IF(K43&lt;=C43, IF(K43&lt;H42,$A$2,IF(K43&lt;H43,$A$3, IF(K43&lt;H44,$A$4, IF(K43&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8642,7 +8591,7 @@
       <c r="J44" s="57"/>
       <c r="K44" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>78.502667212885257</v>
+        <v>39.572896864469044</v>
       </c>
       <c r="L44" s="57" t="str">
         <f ca="1">IF(K44&lt;=C44, IF(K44&lt;H42,$A$2,IF(K44&lt;H43,$A$3, IF(K44&lt;H44,$A$4, IF(K44&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8693,11 +8642,11 @@
       <c r="J45" s="57"/>
       <c r="K45" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>48.751119736986162</v>
+        <v>14.177440051887647</v>
       </c>
       <c r="L45" s="57" t="str">
         <f ca="1">IF(K45&lt;=C45, IF(K45&lt;H42,$A$2,IF(K45&lt;H43,$A$3, IF(K45&lt;H44,$A$4, IF(K45&lt;H45,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_UNCOMMON</v>
       </c>
       <c r="M45" s="57"/>
       <c r="N45" s="57"/>
@@ -8742,7 +8691,7 @@
       </c>
       <c r="K46" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>81.68858631838809</v>
+        <v>77.59684119663099</v>
       </c>
       <c r="L46" s="57" t="str">
         <f ca="1">IF(K46&lt;=C46, IF(K46&lt;H46,$A$2,IF(K46&lt;H47,$A$3, IF(K46&lt;H48,$A$4, IF(K46&lt;H49,$A$5, "NONE")))), "NONE")</f>
@@ -8783,7 +8732,7 @@
       </c>
       <c r="K47" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>24.936317246893836</v>
+        <v>65.346810648663094</v>
       </c>
       <c r="L47" s="57" t="str">
         <f ca="1">IF(K47&lt;=C47, IF(K47&lt;H46,$A$2,IF(K47&lt;H47,$A$3, IF(K47&lt;H48,$A$4, IF(K47&lt;H49,$A$5, "NONE")))), "NONE")</f>
@@ -8824,7 +8773,7 @@
       </c>
       <c r="K48" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>90.68305257257154</v>
+        <v>43.995031842903146</v>
       </c>
       <c r="L48" s="57" t="str">
         <f ca="1">IF(K48&lt;=C48, IF(K48&lt;H46,$A$2,IF(K48&lt;H47,$A$3, IF(K48&lt;H48,$A$4, IF(K48&lt;H49,$A$5, "NONE")))), "NONE")</f>
@@ -8865,11 +8814,11 @@
       </c>
       <c r="K49" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>80.419319315900921</v>
+        <v>14.381147534120364</v>
       </c>
       <c r="L49" s="57" t="str">
         <f ca="1">IF(K49&lt;=C49, IF(K49&lt;H46,$A$2,IF(K49&lt;H47,$A$3, IF(K49&lt;H48,$A$4, IF(K49&lt;H49,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_UNCOMMON</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
@@ -8908,7 +8857,7 @@
       <c r="J50" s="57"/>
       <c r="K50" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>49.106454645643268</v>
+        <v>98.298958423968728</v>
       </c>
       <c r="L50" s="57" t="str">
         <f ca="1">IF(K50&lt;=C50, IF(K50&lt;H50,$A$2,IF(K50&lt;H51,$A$3, IF(K50&lt;H52,$A$4, IF(K50&lt;H53,$A$5, "NONE")))), "NONE")</f>
@@ -8959,11 +8908,11 @@
       <c r="J51" s="57"/>
       <c r="K51" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>1.5962442130746379</v>
+        <v>83.889473470284699</v>
       </c>
       <c r="L51" s="57" t="str">
         <f ca="1">IF(K51&lt;=C51, IF(K51&lt;H50,$A$2,IF(K51&lt;H51,$A$3, IF(K51&lt;H52,$A$4, IF(K51&lt;H53,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
       <c r="M51" s="57"/>
       <c r="N51" s="57"/>
@@ -9010,7 +8959,7 @@
       <c r="J52" s="57"/>
       <c r="K52" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>42.902908034702691</v>
+        <v>92.192012769990853</v>
       </c>
       <c r="L52" s="57" t="str">
         <f ca="1">IF(K52&lt;=C52, IF(K52&lt;H50,$A$2,IF(K52&lt;H51,$A$3, IF(K52&lt;H52,$A$4, IF(K52&lt;H53,$A$5, "NONE")))), "NONE")</f>
@@ -9061,11 +9010,11 @@
       <c r="J53" s="57"/>
       <c r="K53" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>13.204076659853104</v>
+        <v>62.006601587308275</v>
       </c>
       <c r="L53" s="57" t="str">
         <f ca="1">IF(K53&lt;=C53, IF(K53&lt;H50,$A$2,IF(K53&lt;H51,$A$3, IF(K53&lt;H52,$A$4, IF(K53&lt;H53,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
       <c r="M53" s="57"/>
       <c r="N53" s="57"/>
@@ -9110,7 +9059,7 @@
       </c>
       <c r="K54" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>90.676644614504355</v>
+        <v>66.109241819927391</v>
       </c>
       <c r="L54" s="57" t="str">
         <f ca="1">IF(K54&lt;=C54, IF(K54&lt;H54,$A$2,IF(K54&lt;H55,$A$3, IF(K54&lt;H56,$A$4, IF(K54&lt;H57,$A$5, "NONE")))), "NONE")</f>
@@ -9151,11 +9100,11 @@
       </c>
       <c r="K55" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>9.8941852385960534</v>
+        <v>92.219499285570237</v>
       </c>
       <c r="L55" s="57" t="str">
         <f ca="1">IF(K55&lt;=C55, IF(K55&lt;H54,$A$2,IF(K55&lt;H55,$A$3, IF(K55&lt;H56,$A$4, IF(K55&lt;H57,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
@@ -9192,7 +9141,7 @@
       </c>
       <c r="K56" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>28.394175787152221</v>
+        <v>66.439863070893693</v>
       </c>
       <c r="L56" s="57" t="str">
         <f ca="1">IF(K56&lt;=C56, IF(K56&lt;H54,$A$2,IF(K56&lt;H55,$A$3, IF(K56&lt;H56,$A$4, IF(K56&lt;H57,$A$5, "NONE")))), "NONE")</f>
@@ -9233,11 +9182,11 @@
       </c>
       <c r="K57" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>11.799051991309462</v>
+        <v>84.173616550683121</v>
       </c>
       <c r="L57" s="57" t="str">
         <f ca="1">IF(K57&lt;=C57, IF(K57&lt;H54,$A$2,IF(K57&lt;H55,$A$3, IF(K57&lt;H56,$A$4, IF(K57&lt;H57,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
@@ -9276,7 +9225,7 @@
       <c r="J58" s="57"/>
       <c r="K58" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>77.22007459415417</v>
+        <v>65.192487027023233</v>
       </c>
       <c r="L58" s="57" t="str">
         <f ca="1">IF(K58&lt;=C58, IF(K58&lt;H58,$A$2,IF(K58&lt;H59,$A$3, IF(K58&lt;H60,$A$4, IF(K58&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -9327,7 +9276,7 @@
       <c r="J59" s="57"/>
       <c r="K59" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>74.912439673375445</v>
+        <v>82.475532437632111</v>
       </c>
       <c r="L59" s="57" t="str">
         <f ca="1">IF(K59&lt;=C59, IF(K59&lt;H58,$A$2,IF(K59&lt;H59,$A$3, IF(K59&lt;H60,$A$4, IF(K59&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -9378,7 +9327,7 @@
       <c r="J60" s="57"/>
       <c r="K60" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>71.430300842516516</v>
+        <v>98.812513493284385</v>
       </c>
       <c r="L60" s="57" t="str">
         <f ca="1">IF(K60&lt;=C60, IF(K60&lt;H58,$A$2,IF(K60&lt;H59,$A$3, IF(K60&lt;H60,$A$4, IF(K60&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -9429,7 +9378,7 @@
       <c r="J61" s="57"/>
       <c r="K61" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>70.686486323508191</v>
+        <v>81.239877058498635</v>
       </c>
       <c r="L61" s="57" t="str">
         <f ca="1">IF(K61&lt;=C61, IF(K61&lt;H58,$A$2,IF(K61&lt;H59,$A$3, IF(K61&lt;H60,$A$4, IF(K61&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -9478,7 +9427,7 @@
       </c>
       <c r="K62" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>98.736129185611404</v>
+        <v>88.720870554523287</v>
       </c>
       <c r="L62" s="57" t="str">
         <f ca="1">IF(K62&lt;=C62, IF(K62&lt;H62,$A$2,IF(K62&lt;H63,$A$3, IF(K62&lt;H64,$A$4, IF(K62&lt;H65,$A$5, "NONE")))), "NONE")</f>
@@ -9519,7 +9468,7 @@
       </c>
       <c r="K63" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>74.740436415698113</v>
+        <v>72.991544807467193</v>
       </c>
       <c r="L63" s="57" t="str">
         <f ca="1">IF(K63&lt;=C63, IF(K63&lt;H62,$A$2,IF(K63&lt;H63,$A$3, IF(K63&lt;H64,$A$4, IF(K63&lt;H65,$A$5, "NONE")))), "NONE")</f>
@@ -9560,11 +9509,11 @@
       </c>
       <c r="K64" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>1.4427891974466034</v>
+        <v>90.08265733298515</v>
       </c>
       <c r="L64" s="57" t="str">
         <f ca="1">IF(K64&lt;=C64, IF(K64&lt;H62,$A$2,IF(K64&lt;H63,$A$3, IF(K64&lt;H64,$A$4, IF(K64&lt;H65,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
@@ -9601,7 +9550,7 @@
       </c>
       <c r="K65" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>94.257673456681985</v>
+        <v>82.598388558734285</v>
       </c>
       <c r="L65" s="57" t="str">
         <f ca="1">IF(K65&lt;=C65, IF(K65&lt;H62,$A$2,IF(K65&lt;H63,$A$3, IF(K65&lt;H64,$A$4, IF(K65&lt;H65,$A$5, "NONE")))), "NONE")</f>
@@ -9644,7 +9593,7 @@
       <c r="J66" s="57"/>
       <c r="K66" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>58.344351988736342</v>
+        <v>65.374534054135523</v>
       </c>
       <c r="L66" s="57" t="str">
         <f ca="1">IF(K66&lt;=C66, IF(K66&lt;H66,$A$2,IF(K66&lt;H67,$A$3, IF(K66&lt;H68,$A$4, IF(K66&lt;H69,$A$5, "NONE")))), "NONE")</f>
@@ -9695,11 +9644,11 @@
       <c r="J67" s="57"/>
       <c r="K67" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>58.23399556844894</v>
+        <v>29.336485014886815</v>
       </c>
       <c r="L67" s="57" t="str">
         <f ca="1">IF(K67&lt;=C67, IF(K67&lt;H66,$A$2,IF(K67&lt;H67,$A$3, IF(K67&lt;H68,$A$4, IF(K67&lt;H69,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_COMMON</v>
       </c>
       <c r="M67" s="57"/>
       <c r="N67" s="57"/>
@@ -9746,11 +9695,11 @@
       <c r="J68" s="57"/>
       <c r="K68" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>37.04919455479839</v>
+        <v>6.616454908876479</v>
       </c>
       <c r="L68" s="57" t="str">
         <f ca="1">IF(K68&lt;=C68, IF(K68&lt;H66,$A$2,IF(K68&lt;H67,$A$3, IF(K68&lt;H68,$A$4, IF(K68&lt;H69,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
       <c r="M68" s="57"/>
       <c r="N68" s="57"/>
@@ -9797,7 +9746,7 @@
       <c r="J69" s="57"/>
       <c r="K69" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>38.582191796131596</v>
+        <v>61.163393356610918</v>
       </c>
       <c r="L69" s="57" t="str">
         <f ca="1">IF(K69&lt;=C69, IF(K69&lt;H66,$A$2,IF(K69&lt;H67,$A$3, IF(K69&lt;H68,$A$4, IF(K69&lt;H69,$A$5, "NONE")))), "NONE")</f>
@@ -9847,7 +9796,7 @@
       </c>
       <c r="K70" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>61.770402653153496</v>
+        <v>94.824885646684237</v>
       </c>
       <c r="L70" s="57" t="str">
         <f ca="1">IF(K70&lt;=C70, IF(K70&lt;H70,$A$2,IF(K70&lt;H71,$A$3, IF(K70&lt;H72,$A$4, IF(K70&lt;H73,$A$5, "NONE")))), "NONE")</f>
@@ -9889,7 +9838,7 @@
       </c>
       <c r="K71" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>22.278998477260913</v>
+        <v>21.869049151348964</v>
       </c>
       <c r="L71" s="57" t="str">
         <f ca="1">IF(K71&lt;=C71, IF(K71&lt;H70,$A$2,IF(K71&lt;H71,$A$3, IF(K71&lt;H72,$A$4, IF(K71&lt;H73,$A$5, "NONE")))), "NONE")</f>
@@ -9931,11 +9880,11 @@
       </c>
       <c r="K72" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>0.81783909333309479</v>
+        <v>43.943824487470941</v>
       </c>
       <c r="L72" s="57" t="str">
         <f ca="1">IF(K72&lt;=C72, IF(K72&lt;H70,$A$2,IF(K72&lt;H71,$A$3, IF(K72&lt;H72,$A$4, IF(K72&lt;H73,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RELIC</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.2">
@@ -9973,7 +9922,7 @@
       </c>
       <c r="K73" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>82.612893028857471</v>
+        <v>35.288735223440867</v>
       </c>
       <c r="L73" s="57" t="str">
         <f ca="1">IF(K73&lt;=C73, IF(K73&lt;H70,$A$2,IF(K73&lt;H71,$A$3, IF(K73&lt;H72,$A$4, IF(K73&lt;H73,$A$5, "NONE")))), "NONE")</f>
@@ -10017,7 +9966,7 @@
       <c r="J74" s="57"/>
       <c r="K74" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>84.199927960763304</v>
+        <v>97.651282713603138</v>
       </c>
       <c r="L74" s="57" t="str">
         <f ca="1">IF(K74&lt;=C74, IF(K74&lt;H74,$A$2,IF(K74&lt;H75,$A$3, IF(K74&lt;H76,$A$4, IF(K74&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -10069,7 +10018,7 @@
       <c r="J75" s="57"/>
       <c r="K75" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>53.292765689208608</v>
+        <v>63.86432985401661</v>
       </c>
       <c r="L75" s="57" t="str">
         <f ca="1">IF(K75&lt;=C75, IF(K75&lt;H74,$A$2,IF(K75&lt;H75,$A$3, IF(K75&lt;H76,$A$4, IF(K75&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -10121,7 +10070,7 @@
       <c r="J76" s="57"/>
       <c r="K76" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>95.632211197528378</v>
+        <v>32.254928920597024</v>
       </c>
       <c r="L76" s="57" t="str">
         <f ca="1">IF(K76&lt;=C76, IF(K76&lt;H74,$A$2,IF(K76&lt;H75,$A$3, IF(K76&lt;H76,$A$4, IF(K76&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -10173,11 +10122,11 @@
       <c r="J77" s="57"/>
       <c r="K77" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>12.124879339608208</v>
+        <v>40.619968839608944</v>
       </c>
       <c r="L77" s="57" t="str">
         <f ca="1">IF(K77&lt;=C77, IF(K77&lt;H74,$A$2,IF(K77&lt;H75,$A$3, IF(K77&lt;H76,$A$4, IF(K77&lt;H77,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
       <c r="M77" s="57"/>
       <c r="N77" s="57"/>
@@ -10223,7 +10172,7 @@
       </c>
       <c r="K78" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>74.560824413462797</v>
+        <v>43.306622962422779</v>
       </c>
       <c r="L78" s="57" t="str">
         <f ca="1">IF(K78&lt;=C78, IF(K78&lt;H78,$A$2,IF(K78&lt;H79,$A$3, IF(K78&lt;H80,$A$4, IF(K78&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -10265,11 +10214,11 @@
       </c>
       <c r="K79" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>7.3532691422818486</v>
+        <v>59.468686913785383</v>
       </c>
       <c r="L79" s="57" t="str">
         <f ca="1">IF(K79&lt;=C79, IF(K79&lt;H78,$A$2,IF(K79&lt;H79,$A$3, IF(K79&lt;H80,$A$4, IF(K79&lt;H81,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
@@ -10307,7 +10256,7 @@
       </c>
       <c r="K80" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>48.821652021886472</v>
+        <v>98.206785016261335</v>
       </c>
       <c r="L80" s="57" t="str">
         <f ca="1">IF(K80&lt;=C80, IF(K80&lt;H78,$A$2,IF(K80&lt;H79,$A$3, IF(K80&lt;H80,$A$4, IF(K80&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -10349,7 +10298,7 @@
       </c>
       <c r="K81" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>31.856306528667655</v>
+        <v>52.184925644024673</v>
       </c>
       <c r="L81" s="57" t="str">
         <f ca="1">IF(K81&lt;=C81, IF(K81&lt;H78,$A$2,IF(K81&lt;H79,$A$3, IF(K81&lt;H80,$A$4, IF(K81&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -10393,11 +10342,11 @@
       <c r="J82" s="57"/>
       <c r="K82" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>28.06907391875394</v>
+        <v>79.105893673400445</v>
       </c>
       <c r="L82" s="57" t="str">
         <f ca="1">IF(K82&lt;=C82, IF(K82&lt;H82,$A$2,IF(K82&lt;H83,$A$3, IF(K82&lt;H84,$A$4, IF(K82&lt;H85,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
       <c r="M82" s="57"/>
       <c r="N82" s="57"/>
@@ -10445,7 +10394,7 @@
       <c r="J83" s="57"/>
       <c r="K83" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>40.752562583019561</v>
+        <v>33.976301420815957</v>
       </c>
       <c r="L83" s="57" t="str">
         <f ca="1">IF(K83&lt;=C83, IF(K83&lt;H82,$A$2,IF(K83&lt;H83,$A$3, IF(K83&lt;H84,$A$4, IF(K83&lt;H85,$A$5, "NONE")))), "NONE")</f>
@@ -10497,11 +10446,11 @@
       <c r="J84" s="57"/>
       <c r="K84" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>24.099795267512171</v>
+        <v>66.142692434160992</v>
       </c>
       <c r="L84" s="57" t="str">
         <f ca="1">IF(K84&lt;=C84, IF(K84&lt;H82,$A$2,IF(K84&lt;H83,$A$3, IF(K84&lt;H84,$A$4, IF(K84&lt;H85,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_UNCOMMON</v>
+        <v>NONE</v>
       </c>
       <c r="M84" s="57"/>
       <c r="N84" s="57"/>
@@ -10549,7 +10498,7 @@
       <c r="J85" s="57"/>
       <c r="K85" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>55.44494363579453</v>
+        <v>50.107260374997843</v>
       </c>
       <c r="L85" s="57" t="str">
         <f ca="1">IF(K85&lt;=C85, IF(K85&lt;H82,$A$2,IF(K85&lt;H83,$A$3, IF(K85&lt;H84,$A$4, IF(K85&lt;H85,$A$5, "NONE")))), "NONE")</f>
@@ -10599,7 +10548,7 @@
       </c>
       <c r="K86" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>63.851562801085834</v>
+        <v>70.218358308673729</v>
       </c>
       <c r="L86" s="57" t="str">
         <f ca="1">IF(K86&lt;=C86, IF(K86&lt;H86,$A$2,IF(K86&lt;H87,$A$3, IF(K86&lt;H88,$A$4, IF(K86&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10641,7 +10590,7 @@
       </c>
       <c r="K87" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>51.922158984732313</v>
+        <v>40.663301141822359</v>
       </c>
       <c r="L87" s="57" t="str">
         <f ca="1">IF(K87&lt;=C87, IF(K87&lt;H86,$A$2,IF(K87&lt;H87,$A$3, IF(K87&lt;H88,$A$4, IF(K87&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10683,7 +10632,7 @@
       </c>
       <c r="K88" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>70.04001370640961</v>
+        <v>67.751649355678296</v>
       </c>
       <c r="L88" s="57" t="str">
         <f ca="1">IF(K88&lt;=C88, IF(K88&lt;H86,$A$2,IF(K88&lt;H87,$A$3, IF(K88&lt;H88,$A$4, IF(K88&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10725,11 +10674,11 @@
       </c>
       <c r="K89" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>46.752865065231774</v>
+        <v>25.110958779561756</v>
       </c>
       <c r="L89" s="57" t="str">
         <f ca="1">IF(K89&lt;=C89, IF(K89&lt;H86,$A$2,IF(K89&lt;H87,$A$3, IF(K89&lt;H88,$A$4, IF(K89&lt;H89,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_UNCOMMON</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.2">
@@ -10769,11 +10718,11 @@
       <c r="J90" s="57"/>
       <c r="K90" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9574875028202481</v>
+        <v>12.853587187496696</v>
       </c>
       <c r="L90" s="57" t="str">
         <f ca="1">IF(K90&lt;=C90, IF(K90&lt;H90,$A$2,IF(K90&lt;H91,$A$3, IF(K90&lt;H92,$A$4, IF(K90&lt;H93,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>RP_UNCOMMON</v>
       </c>
       <c r="M90" s="57"/>
       <c r="N90" s="57"/>
@@ -10821,11 +10770,11 @@
       <c r="J91" s="57"/>
       <c r="K91" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>5.1794158996103619</v>
+        <v>31.274730192845201</v>
       </c>
       <c r="L91" s="57" t="str">
         <f ca="1">IF(K91&lt;=C91, IF(K91&lt;H90,$A$2,IF(K91&lt;H91,$A$3, IF(K91&lt;H92,$A$4, IF(K91&lt;H93,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
       <c r="M91" s="57"/>
       <c r="N91" s="57"/>
@@ -10873,7 +10822,7 @@
       <c r="J92" s="57"/>
       <c r="K92" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>91.357413442830222</v>
+        <v>58.96674642679811</v>
       </c>
       <c r="L92" s="57" t="str">
         <f ca="1">IF(K92&lt;=C92, IF(K92&lt;H90,$A$2,IF(K92&lt;H91,$A$3, IF(K92&lt;H92,$A$4, IF(K92&lt;H93,$A$5, "NONE")))), "NONE")</f>
@@ -10925,7 +10874,7 @@
       <c r="J93" s="57"/>
       <c r="K93" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>80.569747406399671</v>
+        <v>82.75992406341183</v>
       </c>
       <c r="L93" s="57" t="str">
         <f ca="1">IF(K93&lt;=C93, IF(K93&lt;H90,$A$2,IF(K93&lt;H91,$A$3, IF(K93&lt;H92,$A$4, IF(K93&lt;H93,$A$5, "NONE")))), "NONE")</f>
@@ -10975,11 +10924,11 @@
       </c>
       <c r="K94" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>33.438802771005683</v>
+        <v>7.5509226624160375</v>
       </c>
       <c r="L94" s="57" t="str">
         <f ca="1">IF(K94&lt;=C94, IF(K94&lt;H94,$A$2,IF(K94&lt;H95,$A$3, IF(K94&lt;H96,$A$4, IF(K94&lt;H97,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
@@ -11017,7 +10966,7 @@
       </c>
       <c r="K95" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>63.774502268269963</v>
+        <v>66.674437533728266</v>
       </c>
       <c r="L95" s="57" t="str">
         <f ca="1">IF(K95&lt;=C95, IF(K95&lt;H94,$A$2,IF(K95&lt;H95,$A$3, IF(K95&lt;H96,$A$4, IF(K95&lt;H97,$A$5, "NONE")))), "NONE")</f>
@@ -11059,7 +11008,7 @@
       </c>
       <c r="K96" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>71.669158529881088</v>
+        <v>70.128443314642951</v>
       </c>
       <c r="L96" s="57" t="str">
         <f ca="1">IF(K96&lt;=C96, IF(K96&lt;H94,$A$2,IF(K96&lt;H95,$A$3, IF(K96&lt;H96,$A$4, IF(K96&lt;H97,$A$5, "NONE")))), "NONE")</f>
@@ -11101,7 +11050,7 @@
       </c>
       <c r="K97" s="58">
         <f t="shared" ca="1" si="2"/>
-        <v>80.858551753042505</v>
+        <v>45.086493165202825</v>
       </c>
       <c r="L97" s="57" t="str">
         <f ca="1">IF(K97&lt;=C97, IF(K97&lt;H94,$A$2,IF(K97&lt;H95,$A$3, IF(K97&lt;H96,$A$4, IF(K97&lt;H97,$A$5, "NONE")))), "NONE")</f>
@@ -13177,7 +13126,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A2:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -13190,52 +13139,46 @@
     <col min="8" max="16384" width="14.42578125" style="60"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="27"/>
       <c r="C2" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="27"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="24" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="27"/>
       <c r="C5" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="27"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" s="24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="27"/>
       <c r="C8" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="27"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C9" s="24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
         <v>51</v>
       </c>
@@ -13246,19 +13189,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" s="29"/>
       <c r="C12" s="35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" s="29"/>
       <c r="C13" s="36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>195</v>
       </c>
@@ -13269,31 +13212,28 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="27"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="27"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C17" s="24" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="27"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C18" s="24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="29"/>
       <c r="C19" s="36" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="30" t="s">
         <v>211</v>
       </c>
@@ -13302,13 +13242,13 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B22" s="29"/>
       <c r="C22" s="36" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="30" t="s">
         <v>220</v>
       </c>
@@ -13319,7 +13259,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
         <v>224</v>
       </c>
@@ -13328,26 +13268,25 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="30"/>
       <c r="B26" s="29"/>
       <c r="C26" s="35" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="30"/>
       <c r="B27" s="29"/>
       <c r="C27" s="36" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="30"/>
       <c r="B28" s="29"/>
-      <c r="C28" s="24"/>
-    </row>
-    <row r="29" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
         <v>230</v>
       </c>
@@ -13358,7 +13297,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="30" t="s">
         <v>234</v>
       </c>
@@ -13367,19 +13306,18 @@
         <v>604</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="27"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C31" s="24" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="29"/>
       <c r="C32" s="38" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="30" t="s">
         <v>252</v>
       </c>
@@ -13390,7 +13328,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="30" t="s">
         <v>257</v>
       </c>
@@ -13399,25 +13337,24 @@
         <v>607</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="27"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C36" s="24" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B37" s="29"/>
       <c r="C37" s="35" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B38" s="29"/>
       <c r="C38" s="36" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="31" t="s">
         <v>163</v>
       </c>
@@ -13428,43 +13365,41 @@
         <v>607</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="27"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C44" s="24" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="27"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C45" s="24" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="29"/>
       <c r="C46" s="35" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="29"/>
       <c r="C47" s="35" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" s="29"/>
       <c r="C48" s="38" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B49" s="29"/>
       <c r="C49" s="38" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="31" t="s">
         <v>293</v>
       </c>
@@ -13475,55 +13410,52 @@
         <v>614</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="27"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C52" s="24" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="27"/>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C53" s="24" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="27"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C54" s="24" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B55" s="29"/>
       <c r="C55" s="35" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B56" s="29"/>
       <c r="C56" s="35" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B57" s="29"/>
       <c r="C57" s="35" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B58" s="29"/>
       <c r="C58" s="38" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B59" s="29"/>
       <c r="C59" s="38" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="31" t="s">
         <v>305</v>
       </c>
@@ -13534,43 +13466,40 @@
         <v>609</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="27"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C62" s="24" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="27"/>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C63" s="24" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="27"/>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C64" s="24" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="65" spans="2:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="29"/>
       <c r="C65" s="35" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="66" spans="2:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="29"/>
       <c r="C66" s="35" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="67" spans="2:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="29"/>
       <c r="C67" s="38" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="2:3" s="60" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="29"/>
       <c r="C68" s="38" t="s">
         <v>320</v>

</xml_diff>

<commit_message>
new loot, re-add uncommon gears, item affixes working
</commit_message>
<xml_diff>
--- a/dev/Items.xlsx
+++ b/dev/Items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Warcraft III\Maps\Zulaman-WE\dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Warcraft III\Maps\Zulaman-WE\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB433554-F5C2-49E2-A86C-B0807FF399CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824BAB33-9F67-4E22-8AFA-B82D7B381EEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,12 +24,12 @@
     <sheet name="BossLoot" sheetId="10" r:id="rId9"/>
     <sheet name="MinionLoot" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="848">
   <si>
     <t>TABLE_SIZE</t>
   </si>
@@ -2456,15 +2456,9 @@
     <t>智力</t>
   </si>
   <si>
-    <t>所有属性</t>
-  </si>
-  <si>
     <t>生命值</t>
   </si>
   <si>
-    <t>法力值</t>
-  </si>
-  <si>
     <t>攻击强度</t>
   </si>
   <si>
@@ -2489,33 +2483,6 @@
     <t>躲闪</t>
   </si>
   <si>
-    <t>of Lion Heart</t>
-  </si>
-  <si>
-    <t>狮心之</t>
-  </si>
-  <si>
-    <t>+5力量</t>
-  </si>
-  <si>
-    <t>+5敏捷</t>
-  </si>
-  <si>
-    <t>of Gorilla</t>
-  </si>
-  <si>
-    <t>巨猿之</t>
-  </si>
-  <si>
-    <t>+5智力</t>
-  </si>
-  <si>
-    <t>of Fox</t>
-  </si>
-  <si>
-    <t>红狐之</t>
-  </si>
-  <si>
     <t>of Brute</t>
   </si>
   <si>
@@ -2555,9 +2522,6 @@
     <t>of Ranger</t>
   </si>
   <si>
-    <t>刽子手之</t>
-  </si>
-  <si>
     <t>of Wizard</t>
   </si>
   <si>
@@ -2576,9 +2540,6 @@
     <t>护卫之</t>
   </si>
   <si>
-    <t>+75生命值</t>
-  </si>
-  <si>
     <t>+1%躲闪几率</t>
   </si>
   <si>
@@ -2720,15 +2681,6 @@
     <t>prefix</t>
   </si>
   <si>
-    <t>5-8力量</t>
-  </si>
-  <si>
-    <t>5-8敏捷</t>
-  </si>
-  <si>
-    <t>5-8智力</t>
-  </si>
-  <si>
     <t>厚重的</t>
   </si>
   <si>
@@ -2747,15 +2699,9 @@
     <t>7-10</t>
   </si>
   <si>
-    <t>8-13</t>
-  </si>
-  <si>
     <t>锋利的</t>
   </si>
   <si>
-    <t>Refined</t>
-  </si>
-  <si>
     <t>敏捷的</t>
   </si>
   <si>
@@ -2772,6 +2718,309 @@
   </si>
   <si>
     <t>Intelligent</t>
+  </si>
+  <si>
+    <t>Sharp</t>
+  </si>
+  <si>
+    <t>耐久的</t>
+  </si>
+  <si>
+    <t>生命的</t>
+  </si>
+  <si>
+    <t>Vibrant</t>
+  </si>
+  <si>
+    <t>Endurable</t>
+  </si>
+  <si>
+    <t>60-90</t>
+  </si>
+  <si>
+    <t>熟练的</t>
+  </si>
+  <si>
+    <t>Skilled</t>
+  </si>
+  <si>
+    <t>7-11</t>
+  </si>
+  <si>
+    <t>附魔的</t>
+  </si>
+  <si>
+    <t>Enchanted</t>
+  </si>
+  <si>
+    <t>法术的</t>
+  </si>
+  <si>
+    <t>Sorcerous</t>
+  </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>91-150</t>
+  </si>
+  <si>
+    <t>12-18</t>
+  </si>
+  <si>
+    <t>13-20</t>
+  </si>
+  <si>
+    <t>神秘的</t>
+  </si>
+  <si>
+    <t>Mysterious</t>
+  </si>
+  <si>
+    <t>Cruel</t>
+  </si>
+  <si>
+    <t>永恒的</t>
+  </si>
+  <si>
+    <t>Eternal</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>4-5</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5-7</t>
+  </si>
+  <si>
+    <t>护甲</t>
+  </si>
+  <si>
+    <t>稳固的</t>
+  </si>
+  <si>
+    <t>Steady</t>
+  </si>
+  <si>
+    <t>坚硬的</t>
+  </si>
+  <si>
+    <t>Tough</t>
+  </si>
+  <si>
+    <t>3-5</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>of Wind Serpent</t>
+  </si>
+  <si>
+    <t>风蛇之</t>
+  </si>
+  <si>
+    <t>of Snake</t>
+  </si>
+  <si>
+    <t>灵蛇之</t>
+  </si>
+  <si>
+    <t>5-10</t>
+  </si>
+  <si>
+    <t>4-8</t>
+  </si>
+  <si>
+    <t>6-12</t>
+  </si>
+  <si>
+    <t>活力之</t>
+  </si>
+  <si>
+    <t>of Vitality</t>
+  </si>
+  <si>
+    <t>90-180</t>
+  </si>
+  <si>
+    <t>8-11</t>
+  </si>
+  <si>
+    <t>游侠之</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>70-100</t>
+  </si>
+  <si>
+    <t>精通之</t>
+  </si>
+  <si>
+    <t>of Mastery</t>
+  </si>
+  <si>
+    <t>模糊之</t>
+  </si>
+  <si>
+    <t>of Blur</t>
+  </si>
+  <si>
+    <t>堡垒之</t>
+  </si>
+  <si>
+    <t>of Stronghold</t>
+  </si>
+  <si>
+    <t>深海之</t>
+  </si>
+  <si>
+    <t>of Deep Sea</t>
+  </si>
+  <si>
+    <t>3-6</t>
+  </si>
+  <si>
+    <t>虚空之</t>
+  </si>
+  <si>
+    <t>of Void</t>
+  </si>
+  <si>
+    <t>12-24</t>
+  </si>
+  <si>
+    <t>of Quickness</t>
+  </si>
+  <si>
+    <t>致命之</t>
+  </si>
+  <si>
+    <t>of Lethality</t>
+  </si>
+  <si>
+    <t>快速之</t>
+  </si>
+  <si>
+    <t>残忍的</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
   </si>
 </sst>
 </file>
@@ -2969,20 +3218,22 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.5"/>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="微软雅黑"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3012,6 +3263,18 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3026,7 +3289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3189,19 +3452,25 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="29" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="29" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -6294,7 +6563,7 @@
       <c r="J2" s="69"/>
       <c r="K2" s="70">
         <f t="shared" ref="K2:K97" ca="1" si="2">RAND() * 100</f>
-        <v>70.500284380012985</v>
+        <v>9.7973208702744294</v>
       </c>
       <c r="L2" s="69" t="str">
         <f ca="1">IF(K2&lt;=C2, IF(K2&lt;H2,$A$2,IF(K2&lt;H3,$A$3, IF(K2&lt;H4,$A$4, IF(K2&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6347,7 +6616,7 @@
       <c r="J3" s="69"/>
       <c r="K3" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>56.524556057939165</v>
+        <v>42.675830044316896</v>
       </c>
       <c r="L3" s="69" t="str">
         <f ca="1">IF(K3&lt;=C3, IF(K3&lt;H2,$A$2,IF(K3&lt;H3,$A$3, IF(K3&lt;H4,$A$4, IF(K3&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6400,7 +6669,7 @@
       <c r="J4" s="69"/>
       <c r="K4" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>83.373974588202643</v>
+        <v>43.338946279768862</v>
       </c>
       <c r="L4" s="69" t="str">
         <f ca="1">IF(K4&lt;=C4, IF(K4&lt;H2,$A$2,IF(K4&lt;H3,$A$3, IF(K4&lt;H4,$A$4, IF(K4&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6453,7 +6722,7 @@
       <c r="J5" s="69"/>
       <c r="K5" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>76.038608482829403</v>
+        <v>50.397229744380176</v>
       </c>
       <c r="L5" s="69" t="str">
         <f ca="1">IF(K5&lt;=C5, IF(K5&lt;H2,$A$2,IF(K5&lt;H3,$A$3, IF(K5&lt;H4,$A$4, IF(K5&lt;H5,$A$5, "NONE")))), "NONE")</f>
@@ -6503,7 +6772,7 @@
       </c>
       <c r="K6" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>64.080814774618133</v>
+        <v>18.223184733406718</v>
       </c>
       <c r="L6" s="69" t="str">
         <f ca="1">IF(K6&lt;=C6, IF(K6&lt;H6,$A$2,IF(K6&lt;H7,$A$3, IF(K6&lt;H8,$A$4, IF(K6&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -6545,7 +6814,7 @@
       </c>
       <c r="K7" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>32.973065131582388</v>
+        <v>56.539055022924892</v>
       </c>
       <c r="L7" s="69" t="str">
         <f ca="1">IF(K7&lt;=C7, IF(K7&lt;H6,$A$2,IF(K7&lt;H7,$A$3, IF(K7&lt;H8,$A$4, IF(K7&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -6587,7 +6856,7 @@
       </c>
       <c r="K8" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>21.838748671248197</v>
+        <v>32.087559064922729</v>
       </c>
       <c r="L8" s="69" t="str">
         <f ca="1">IF(K8&lt;=C8, IF(K8&lt;H6,$A$2,IF(K8&lt;H7,$A$3, IF(K8&lt;H8,$A$4, IF(K8&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -6629,7 +6898,7 @@
       </c>
       <c r="K9" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>64.051984342370332</v>
+        <v>54.726625542009465</v>
       </c>
       <c r="L9" s="69" t="str">
         <f ca="1">IF(K9&lt;=C9, IF(K9&lt;H6,$A$2,IF(K9&lt;H7,$A$3, IF(K9&lt;H8,$A$4, IF(K9&lt;H9,$A$5, "NONE")))), "NONE")</f>
@@ -6673,7 +6942,7 @@
       <c r="J10" s="69"/>
       <c r="K10" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>12.154550722296232</v>
+        <v>50.22140408811542</v>
       </c>
       <c r="L10" s="69" t="str">
         <f ca="1">IF(K10&lt;=C10, IF(K10&lt;H10,$A$2,IF(K10&lt;H11,$A$3, IF(K10&lt;H12,$A$4, IF(K10&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -6725,7 +6994,7 @@
       <c r="J11" s="69"/>
       <c r="K11" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>38.270898855798393</v>
+        <v>50.110473032712669</v>
       </c>
       <c r="L11" s="69" t="str">
         <f ca="1">IF(K11&lt;=C11, IF(K11&lt;H10,$A$2,IF(K11&lt;H11,$A$3, IF(K11&lt;H12,$A$4, IF(K11&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -6777,7 +7046,7 @@
       <c r="J12" s="69"/>
       <c r="K12" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>53.345556484318003</v>
+        <v>13.998734961456183</v>
       </c>
       <c r="L12" s="69" t="str">
         <f ca="1">IF(K12&lt;=C12, IF(K12&lt;H10,$A$2,IF(K12&lt;H11,$A$3, IF(K12&lt;H12,$A$4, IF(K12&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -6829,7 +7098,7 @@
       <c r="J13" s="69"/>
       <c r="K13" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>68.962877483555147</v>
+        <v>74.610531645383887</v>
       </c>
       <c r="L13" s="69" t="str">
         <f ca="1">IF(K13&lt;=C13, IF(K13&lt;H10,$A$2,IF(K13&lt;H11,$A$3, IF(K13&lt;H12,$A$4, IF(K13&lt;H13,$A$5, "NONE")))), "NONE")</f>
@@ -6879,7 +7148,7 @@
       </c>
       <c r="K14" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>14.614194682991554</v>
+        <v>22.311374971298125</v>
       </c>
       <c r="L14" s="69" t="str">
         <f ca="1">IF(K14&lt;=C14, IF(K14&lt;H14,$A$2,IF(K14&lt;H15,$A$3, IF(K14&lt;H16,$A$4, IF(K14&lt;H17,$A$5, "NONE")))), "NONE")</f>
@@ -6921,7 +7190,7 @@
       </c>
       <c r="K15" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>29.22052140039678</v>
+        <v>6.032445603983005</v>
       </c>
       <c r="L15" s="69" t="str">
         <f ca="1">IF(K15&lt;=C15, IF(K15&lt;H14,$A$2,IF(K15&lt;H15,$A$3, IF(K15&lt;H16,$A$4, IF(K15&lt;H17,$A$5, "NONE")))), "NONE")</f>
@@ -6963,7 +7232,7 @@
       </c>
       <c r="K16" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>70.659509763557892</v>
+        <v>88.621456941621204</v>
       </c>
       <c r="L16" s="69" t="str">
         <f ca="1">IF(K16&lt;=C16, IF(K16&lt;H14,$A$2,IF(K16&lt;H15,$A$3, IF(K16&lt;H16,$A$4, IF(K16&lt;H17,$A$5, "NONE")))), "NONE")</f>
@@ -7005,7 +7274,7 @@
       </c>
       <c r="K17" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>21.3763832115642</v>
+        <v>61.890491068169609</v>
       </c>
       <c r="L17" s="69" t="str">
         <f ca="1">IF(K17&lt;=C17, IF(K17&lt;H14,$A$2,IF(K17&lt;H15,$A$3, IF(K17&lt;H16,$A$4, IF(K17&lt;H17,$A$5, "NONE")))), "NONE")</f>
@@ -7049,11 +7318,11 @@
       <c r="J18" s="69"/>
       <c r="K18" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2495482317702589</v>
+        <v>44.810134954219237</v>
       </c>
       <c r="L18" s="69" t="str">
         <f ca="1">IF(K18&lt;=C18, IF(K18&lt;H18,$A$2,IF(K18&lt;H19,$A$3, IF(K18&lt;H20,$A$4, IF(K18&lt;H21,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
       <c r="M18" s="69"/>
       <c r="N18" s="69"/>
@@ -7101,7 +7370,7 @@
       <c r="J19" s="69"/>
       <c r="K19" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>33.400931045939508</v>
+        <v>84.181631841792736</v>
       </c>
       <c r="L19" s="69" t="str">
         <f ca="1">IF(K19&lt;=C19, IF(K19&lt;H18,$A$2,IF(K19&lt;H19,$A$3, IF(K19&lt;H20,$A$4, IF(K19&lt;H21,$A$5, "NONE")))), "NONE")</f>
@@ -7153,11 +7422,11 @@
       <c r="J20" s="69"/>
       <c r="K20" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>67.33365807634037</v>
+        <v>1.606894201611786</v>
       </c>
       <c r="L20" s="69" t="str">
         <f ca="1">IF(K20&lt;=C20, IF(K20&lt;H18,$A$2,IF(K20&lt;H19,$A$3, IF(K20&lt;H20,$A$4, IF(K20&lt;H21,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
       <c r="M20" s="69"/>
       <c r="N20" s="69"/>
@@ -7205,7 +7474,7 @@
       <c r="J21" s="69"/>
       <c r="K21" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>95.132938035521491</v>
+        <v>4.2095353619608034</v>
       </c>
       <c r="L21" s="69" t="str">
         <f ca="1">IF(K21&lt;=C21, IF(K21&lt;H18,$A$2,IF(K21&lt;H19,$A$3, IF(K21&lt;H20,$A$4, IF(K21&lt;H21,$A$5, "NONE")))), "NONE")</f>
@@ -7255,7 +7524,7 @@
       </c>
       <c r="K22" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>46.113907267176401</v>
+        <v>91.567530023456925</v>
       </c>
       <c r="L22" s="69" t="str">
         <f ca="1">IF(K22&lt;=C22, IF(K22&lt;H22,$A$2,IF(K22&lt;H23,$A$3, IF(K22&lt;H24,$A$4, IF(K22&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7297,7 +7566,7 @@
       </c>
       <c r="K23" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>90.473861724866794</v>
+        <v>5.7053630454815485</v>
       </c>
       <c r="L23" s="69" t="str">
         <f ca="1">IF(K23&lt;=C23, IF(K23&lt;H22,$A$2,IF(K23&lt;H23,$A$3, IF(K23&lt;H24,$A$4, IF(K23&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7339,7 +7608,7 @@
       </c>
       <c r="K24" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>99.197555711131542</v>
+        <v>27.894230073383486</v>
       </c>
       <c r="L24" s="69" t="str">
         <f ca="1">IF(K24&lt;=C24, IF(K24&lt;H22,$A$2,IF(K24&lt;H23,$A$3, IF(K24&lt;H24,$A$4, IF(K24&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7381,7 +7650,7 @@
       </c>
       <c r="K25" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>52.95338932764836</v>
+        <v>27.063510536172508</v>
       </c>
       <c r="L25" s="69" t="str">
         <f ca="1">IF(K25&lt;=C25, IF(K25&lt;H22,$A$2,IF(K25&lt;H23,$A$3, IF(K25&lt;H24,$A$4, IF(K25&lt;H25,$A$5, "NONE")))), "NONE")</f>
@@ -7425,7 +7694,7 @@
       <c r="J26" s="69"/>
       <c r="K26" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>7.8311181564264203</v>
+        <v>37.265068912549992</v>
       </c>
       <c r="L26" s="69" t="str">
         <f ca="1">IF(K26&lt;=C26, IF(K26&lt;H26,$A$2,IF(K26&lt;H27,$A$3, IF(K26&lt;H28,$A$4, IF(K26&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7477,7 +7746,7 @@
       <c r="J27" s="69"/>
       <c r="K27" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>85.531021788454595</v>
+        <v>62.859671619729482</v>
       </c>
       <c r="L27" s="69" t="str">
         <f ca="1">IF(K27&lt;=C27, IF(K27&lt;H26,$A$2,IF(K27&lt;H27,$A$3, IF(K27&lt;H28,$A$4, IF(K27&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7529,7 +7798,7 @@
       <c r="J28" s="69"/>
       <c r="K28" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>50.564733419369915</v>
+        <v>71.359129734580605</v>
       </c>
       <c r="L28" s="69" t="str">
         <f ca="1">IF(K28&lt;=C28, IF(K28&lt;H26,$A$2,IF(K28&lt;H27,$A$3, IF(K28&lt;H28,$A$4, IF(K28&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7581,7 +7850,7 @@
       <c r="J29" s="69"/>
       <c r="K29" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>82.36714675292292</v>
+        <v>69.011550874827023</v>
       </c>
       <c r="L29" s="69" t="str">
         <f ca="1">IF(K29&lt;=C29, IF(K29&lt;H26,$A$2,IF(K29&lt;H27,$A$3, IF(K29&lt;H28,$A$4, IF(K29&lt;H29,$A$5, "NONE")))), "NONE")</f>
@@ -7631,7 +7900,7 @@
       </c>
       <c r="K30" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>46.161962142343619</v>
+        <v>46.978318859066903</v>
       </c>
       <c r="L30" s="69" t="str">
         <f ca="1">IF(K30&lt;=C30, IF(K30&lt;H30,$A$2,IF(K30&lt;H31,$A$3, IF(K30&lt;H32,$A$4, IF(K30&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -7673,7 +7942,7 @@
       </c>
       <c r="K31" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>29.900079709557158</v>
+        <v>12.764703574924141</v>
       </c>
       <c r="L31" s="69" t="str">
         <f ca="1">IF(K31&lt;=C31, IF(K31&lt;H30,$A$2,IF(K31&lt;H31,$A$3, IF(K31&lt;H32,$A$4, IF(K31&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -7715,7 +7984,7 @@
       </c>
       <c r="K32" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>50.566592966203629</v>
+        <v>29.453069337022043</v>
       </c>
       <c r="L32" s="69" t="str">
         <f ca="1">IF(K32&lt;=C32, IF(K32&lt;H30,$A$2,IF(K32&lt;H31,$A$3, IF(K32&lt;H32,$A$4, IF(K32&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -7757,7 +8026,7 @@
       </c>
       <c r="K33" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>41.002067701173203</v>
+        <v>56.688120027038813</v>
       </c>
       <c r="L33" s="69" t="str">
         <f ca="1">IF(K33&lt;=C33, IF(K33&lt;H30,$A$2,IF(K33&lt;H31,$A$3, IF(K33&lt;H32,$A$4, IF(K33&lt;H33,$A$5, "NONE")))), "NONE")</f>
@@ -7801,11 +8070,11 @@
       <c r="J34" s="69"/>
       <c r="K34" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>68.351324876599932</v>
+        <v>1.8632959378783065</v>
       </c>
       <c r="L34" s="69" t="str">
         <f ca="1">IF(K34&lt;=C34, IF(K34&lt;H34,$A$2,IF(K34&lt;H35,$A$3, IF(K34&lt;H36,$A$4, IF(K34&lt;H37,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
       <c r="M34" s="69"/>
       <c r="N34" s="69"/>
@@ -7853,7 +8122,7 @@
       <c r="J35" s="69"/>
       <c r="K35" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>35.905400995710082</v>
+        <v>83.627159594358886</v>
       </c>
       <c r="L35" s="69" t="str">
         <f ca="1">IF(K35&lt;=C35, IF(K35&lt;H34,$A$2,IF(K35&lt;H35,$A$3, IF(K35&lt;H36,$A$4, IF(K35&lt;H37,$A$5, "NONE")))), "NONE")</f>
@@ -7905,7 +8174,7 @@
       <c r="J36" s="69"/>
       <c r="K36" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>53.823004612167978</v>
+        <v>23.158749545165048</v>
       </c>
       <c r="L36" s="69" t="str">
         <f ca="1">IF(K36&lt;=C36, IF(K36&lt;H34,$A$2,IF(K36&lt;H35,$A$3, IF(K36&lt;H36,$A$4, IF(K36&lt;H37,$A$5, "NONE")))), "NONE")</f>
@@ -7957,7 +8226,7 @@
       <c r="J37" s="69"/>
       <c r="K37" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>74.754957977767845</v>
+        <v>35.958151513897853</v>
       </c>
       <c r="L37" s="69" t="str">
         <f ca="1">IF(K37&lt;=C37, IF(K37&lt;H34,$A$2,IF(K37&lt;H35,$A$3, IF(K37&lt;H36,$A$4, IF(K37&lt;H37,$A$5, "NONE")))), "NONE")</f>
@@ -8007,7 +8276,7 @@
       </c>
       <c r="K38" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>73.674908930889302</v>
+        <v>75.663584641597538</v>
       </c>
       <c r="L38" s="69" t="str">
         <f ca="1">IF(K38&lt;=C38, IF(K38&lt;H38,$A$2,IF(K38&lt;H39,$A$3, IF(K38&lt;H40,$A$4, IF(K38&lt;H41,$A$5, "NONE")))), "NONE")</f>
@@ -8049,7 +8318,7 @@
       </c>
       <c r="K39" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>47.004268379861138</v>
+        <v>53.45056209011414</v>
       </c>
       <c r="L39" s="69" t="str">
         <f ca="1">IF(K39&lt;=C39, IF(K39&lt;H38,$A$2,IF(K39&lt;H39,$A$3, IF(K39&lt;H40,$A$4, IF(K39&lt;H41,$A$5, "NONE")))), "NONE")</f>
@@ -8091,7 +8360,7 @@
       </c>
       <c r="K40" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>70.519313562949833</v>
+        <v>96.175073081962751</v>
       </c>
       <c r="L40" s="69" t="str">
         <f ca="1">IF(K40&lt;=C40, IF(K40&lt;H38,$A$2,IF(K40&lt;H39,$A$3, IF(K40&lt;H40,$A$4, IF(K40&lt;H41,$A$5, "NONE")))), "NONE")</f>
@@ -8133,11 +8402,11 @@
       </c>
       <c r="K41" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>41.525955007403006</v>
+        <v>0.62474092602166076</v>
       </c>
       <c r="L41" s="69" t="str">
         <f ca="1">IF(K41&lt;=C41, IF(K41&lt;H38,$A$2,IF(K41&lt;H39,$A$3, IF(K41&lt;H40,$A$4, IF(K41&lt;H41,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -8177,7 +8446,7 @@
       <c r="J42" s="69"/>
       <c r="K42" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>67.852550991078743</v>
+        <v>64.611185509108608</v>
       </c>
       <c r="L42" s="69" t="str">
         <f ca="1">IF(K42&lt;=C42, IF(K42&lt;H42,$A$2,IF(K42&lt;H43,$A$3, IF(K42&lt;H44,$A$4, IF(K42&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8229,7 +8498,7 @@
       <c r="J43" s="69"/>
       <c r="K43" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>5.4663363433678613</v>
+        <v>5.8113154952290973</v>
       </c>
       <c r="L43" s="69" t="str">
         <f ca="1">IF(K43&lt;=C43, IF(K43&lt;H42,$A$2,IF(K43&lt;H43,$A$3, IF(K43&lt;H44,$A$4, IF(K43&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8281,7 +8550,7 @@
       <c r="J44" s="69"/>
       <c r="K44" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>14.743335011688874</v>
+        <v>29.933407924199763</v>
       </c>
       <c r="L44" s="69" t="str">
         <f ca="1">IF(K44&lt;=C44, IF(K44&lt;H42,$A$2,IF(K44&lt;H43,$A$3, IF(K44&lt;H44,$A$4, IF(K44&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8333,7 +8602,7 @@
       <c r="J45" s="69"/>
       <c r="K45" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>91.085659218439787</v>
+        <v>53.920251912112228</v>
       </c>
       <c r="L45" s="69" t="str">
         <f ca="1">IF(K45&lt;=C45, IF(K45&lt;H42,$A$2,IF(K45&lt;H43,$A$3, IF(K45&lt;H44,$A$4, IF(K45&lt;H45,$A$5, "NONE")))), "NONE")</f>
@@ -8383,7 +8652,7 @@
       </c>
       <c r="K46" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>12.711532117033286</v>
+        <v>57.747919994373461</v>
       </c>
       <c r="L46" s="69" t="str">
         <f ca="1">IF(K46&lt;=C46, IF(K46&lt;H46,$A$2,IF(K46&lt;H47,$A$3, IF(K46&lt;H48,$A$4, IF(K46&lt;H49,$A$5, "NONE")))), "NONE")</f>
@@ -8425,11 +8694,11 @@
       </c>
       <c r="K47" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>27.066897411698665</v>
+        <v>1.8758929303932304</v>
       </c>
       <c r="L47" s="69" t="str">
         <f ca="1">IF(K47&lt;=C47, IF(K47&lt;H46,$A$2,IF(K47&lt;H47,$A$3, IF(K47&lt;H48,$A$4, IF(K47&lt;H49,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
@@ -8467,11 +8736,11 @@
       </c>
       <c r="K48" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>0.78926334048957658</v>
+        <v>79.370349462041219</v>
       </c>
       <c r="L48" s="69" t="str">
         <f ca="1">IF(K48&lt;=C48, IF(K48&lt;H46,$A$2,IF(K48&lt;H47,$A$3, IF(K48&lt;H48,$A$4, IF(K48&lt;H49,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
@@ -8509,7 +8778,7 @@
       </c>
       <c r="K49" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>33.891407546983018</v>
+        <v>66.744270566054112</v>
       </c>
       <c r="L49" s="69" t="str">
         <f ca="1">IF(K49&lt;=C49, IF(K49&lt;H46,$A$2,IF(K49&lt;H47,$A$3, IF(K49&lt;H48,$A$4, IF(K49&lt;H49,$A$5, "NONE")))), "NONE")</f>
@@ -8553,7 +8822,7 @@
       <c r="J50" s="69"/>
       <c r="K50" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>49.837804058764988</v>
+        <v>52.324864848881589</v>
       </c>
       <c r="L50" s="69" t="str">
         <f ca="1">IF(K50&lt;=C50, IF(K50&lt;H50,$A$2,IF(K50&lt;H51,$A$3, IF(K50&lt;H52,$A$4, IF(K50&lt;H53,$A$5, "NONE")))), "NONE")</f>
@@ -8605,7 +8874,7 @@
       <c r="J51" s="69"/>
       <c r="K51" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>20.340802271125924</v>
+        <v>15.105011336278285</v>
       </c>
       <c r="L51" s="69" t="str">
         <f ca="1">IF(K51&lt;=C51, IF(K51&lt;H50,$A$2,IF(K51&lt;H51,$A$3, IF(K51&lt;H52,$A$4, IF(K51&lt;H53,$A$5, "NONE")))), "NONE")</f>
@@ -8657,7 +8926,7 @@
       <c r="J52" s="69"/>
       <c r="K52" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>88.689412174095409</v>
+        <v>99.978232544434945</v>
       </c>
       <c r="L52" s="69" t="str">
         <f ca="1">IF(K52&lt;=C52, IF(K52&lt;H50,$A$2,IF(K52&lt;H51,$A$3, IF(K52&lt;H52,$A$4, IF(K52&lt;H53,$A$5, "NONE")))), "NONE")</f>
@@ -8709,7 +8978,7 @@
       <c r="J53" s="69"/>
       <c r="K53" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>54.44337622091826</v>
+        <v>50.52978183018525</v>
       </c>
       <c r="L53" s="69" t="str">
         <f ca="1">IF(K53&lt;=C53, IF(K53&lt;H50,$A$2,IF(K53&lt;H51,$A$3, IF(K53&lt;H52,$A$4, IF(K53&lt;H53,$A$5, "NONE")))), "NONE")</f>
@@ -8759,7 +9028,7 @@
       </c>
       <c r="K54" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>23.179638834354087</v>
+        <v>8.5591891030888831</v>
       </c>
       <c r="L54" s="69" t="str">
         <f ca="1">IF(K54&lt;=C54, IF(K54&lt;H54,$A$2,IF(K54&lt;H55,$A$3, IF(K54&lt;H56,$A$4, IF(K54&lt;H57,$A$5, "NONE")))), "NONE")</f>
@@ -8801,7 +9070,7 @@
       </c>
       <c r="K55" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>22.689039994456696</v>
+        <v>24.767603091100231</v>
       </c>
       <c r="L55" s="69" t="str">
         <f ca="1">IF(K55&lt;=C55, IF(K55&lt;H54,$A$2,IF(K55&lt;H55,$A$3, IF(K55&lt;H56,$A$4, IF(K55&lt;H57,$A$5, "NONE")))), "NONE")</f>
@@ -8843,11 +9112,11 @@
       </c>
       <c r="K56" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>89.744165432127687</v>
+        <v>2.3241145740503399</v>
       </c>
       <c r="L56" s="69" t="str">
         <f ca="1">IF(K56&lt;=C56, IF(K56&lt;H54,$A$2,IF(K56&lt;H55,$A$3, IF(K56&lt;H56,$A$4, IF(K56&lt;H57,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
@@ -8885,11 +9154,11 @@
       </c>
       <c r="K57" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>8.3139634233342701</v>
+        <v>4.7631023389835825</v>
       </c>
       <c r="L57" s="69" t="str">
         <f ca="1">IF(K57&lt;=C57, IF(K57&lt;H54,$A$2,IF(K57&lt;H55,$A$3, IF(K57&lt;H56,$A$4, IF(K57&lt;H57,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
@@ -8929,7 +9198,7 @@
       <c r="J58" s="69"/>
       <c r="K58" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>8.9616019501738027</v>
+        <v>27.38111733969706</v>
       </c>
       <c r="L58" s="69" t="str">
         <f ca="1">IF(K58&lt;=C58, IF(K58&lt;H58,$A$2,IF(K58&lt;H59,$A$3, IF(K58&lt;H60,$A$4, IF(K58&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -8981,7 +9250,7 @@
       <c r="J59" s="69"/>
       <c r="K59" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>8.6412405957916327</v>
+        <v>68.280096719056687</v>
       </c>
       <c r="L59" s="69" t="str">
         <f ca="1">IF(K59&lt;=C59, IF(K59&lt;H58,$A$2,IF(K59&lt;H59,$A$3, IF(K59&lt;H60,$A$4, IF(K59&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -9033,11 +9302,11 @@
       <c r="J60" s="69"/>
       <c r="K60" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>2.0721395292878642</v>
+        <v>50.853164547525807</v>
       </c>
       <c r="L60" s="69" t="str">
         <f ca="1">IF(K60&lt;=C60, IF(K60&lt;H58,$A$2,IF(K60&lt;H59,$A$3, IF(K60&lt;H60,$A$4, IF(K60&lt;H61,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
       <c r="M60" s="69"/>
       <c r="N60" s="69"/>
@@ -9085,7 +9354,7 @@
       <c r="J61" s="69"/>
       <c r="K61" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>4.8060883505642309</v>
+        <v>7.4859728881787486</v>
       </c>
       <c r="L61" s="69" t="str">
         <f ca="1">IF(K61&lt;=C61, IF(K61&lt;H58,$A$2,IF(K61&lt;H59,$A$3, IF(K61&lt;H60,$A$4, IF(K61&lt;H61,$A$5, "NONE")))), "NONE")</f>
@@ -9135,11 +9404,11 @@
       </c>
       <c r="K62" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>6.9561042302823228</v>
+        <v>36.001208242456009</v>
       </c>
       <c r="L62" s="69" t="str">
         <f ca="1">IF(K62&lt;=C62, IF(K62&lt;H62,$A$2,IF(K62&lt;H63,$A$3, IF(K62&lt;H64,$A$4, IF(K62&lt;H65,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
@@ -9177,11 +9446,11 @@
       </c>
       <c r="K63" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>7.7486744292327163</v>
+        <v>82.347633710442295</v>
       </c>
       <c r="L63" s="69" t="str">
         <f ca="1">IF(K63&lt;=C63, IF(K63&lt;H62,$A$2,IF(K63&lt;H63,$A$3, IF(K63&lt;H64,$A$4, IF(K63&lt;H65,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
@@ -9219,7 +9488,7 @@
       </c>
       <c r="K64" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>88.866972995295484</v>
+        <v>14.271215177555408</v>
       </c>
       <c r="L64" s="69" t="str">
         <f ca="1">IF(K64&lt;=C64, IF(K64&lt;H62,$A$2,IF(K64&lt;H63,$A$3, IF(K64&lt;H64,$A$4, IF(K64&lt;H65,$A$5, "NONE")))), "NONE")</f>
@@ -9261,11 +9530,11 @@
       </c>
       <c r="K65" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>7.6464214851558303</v>
+        <v>26.920333266996654</v>
       </c>
       <c r="L65" s="69" t="str">
         <f ca="1">IF(K65&lt;=C65, IF(K65&lt;H62,$A$2,IF(K65&lt;H63,$A$3, IF(K65&lt;H64,$A$4, IF(K65&lt;H65,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
@@ -9305,7 +9574,7 @@
       <c r="J66" s="69"/>
       <c r="K66" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>48.895948652295843</v>
+        <v>99.183468076635535</v>
       </c>
       <c r="L66" s="69" t="str">
         <f ca="1">IF(K66&lt;=C66, IF(K66&lt;H66,$A$2,IF(K66&lt;H67,$A$3, IF(K66&lt;H68,$A$4, IF(K66&lt;H69,$A$5, "NONE")))), "NONE")</f>
@@ -9357,7 +9626,7 @@
       <c r="J67" s="69"/>
       <c r="K67" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>42.902892071450538</v>
+        <v>32.12973997842812</v>
       </c>
       <c r="L67" s="69" t="str">
         <f ca="1">IF(K67&lt;=C67, IF(K67&lt;H66,$A$2,IF(K67&lt;H67,$A$3, IF(K67&lt;H68,$A$4, IF(K67&lt;H69,$A$5, "NONE")))), "NONE")</f>
@@ -9409,7 +9678,7 @@
       <c r="J68" s="69"/>
       <c r="K68" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>64.60887752041674</v>
+        <v>77.865364866049489</v>
       </c>
       <c r="L68" s="69" t="str">
         <f ca="1">IF(K68&lt;=C68, IF(K68&lt;H66,$A$2,IF(K68&lt;H67,$A$3, IF(K68&lt;H68,$A$4, IF(K68&lt;H69,$A$5, "NONE")))), "NONE")</f>
@@ -9461,7 +9730,7 @@
       <c r="J69" s="69"/>
       <c r="K69" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>37.72133163963143</v>
+        <v>86.941349735852043</v>
       </c>
       <c r="L69" s="69" t="str">
         <f ca="1">IF(K69&lt;=C69, IF(K69&lt;H66,$A$2,IF(K69&lt;H67,$A$3, IF(K69&lt;H68,$A$4, IF(K69&lt;H69,$A$5, "NONE")))), "NONE")</f>
@@ -9511,7 +9780,7 @@
       </c>
       <c r="K70" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>50.474188622509317</v>
+        <v>14.710254630193054</v>
       </c>
       <c r="L70" s="69" t="str">
         <f ca="1">IF(K70&lt;=C70, IF(K70&lt;H70,$A$2,IF(K70&lt;H71,$A$3, IF(K70&lt;H72,$A$4, IF(K70&lt;H73,$A$5, "NONE")))), "NONE")</f>
@@ -9553,7 +9822,7 @@
       </c>
       <c r="K71" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>68.475956041757087</v>
+        <v>63.267207176670141</v>
       </c>
       <c r="L71" s="69" t="str">
         <f ca="1">IF(K71&lt;=C71, IF(K71&lt;H70,$A$2,IF(K71&lt;H71,$A$3, IF(K71&lt;H72,$A$4, IF(K71&lt;H73,$A$5, "NONE")))), "NONE")</f>
@@ -9595,7 +9864,7 @@
       </c>
       <c r="K72" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>39.677161079817388</v>
+        <v>11.322415487665104</v>
       </c>
       <c r="L72" s="69" t="str">
         <f ca="1">IF(K72&lt;=C72, IF(K72&lt;H70,$A$2,IF(K72&lt;H71,$A$3, IF(K72&lt;H72,$A$4, IF(K72&lt;H73,$A$5, "NONE")))), "NONE")</f>
@@ -9637,11 +9906,11 @@
       </c>
       <c r="K73" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>7.6730051893220459</v>
+        <v>41.715349696404303</v>
       </c>
       <c r="L73" s="69" t="str">
         <f ca="1">IF(K73&lt;=C73, IF(K73&lt;H70,$A$2,IF(K73&lt;H71,$A$3, IF(K73&lt;H72,$A$4, IF(K73&lt;H73,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
@@ -9681,7 +9950,7 @@
       <c r="J74" s="69"/>
       <c r="K74" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>38.156952546226599</v>
+        <v>56.831934236573808</v>
       </c>
       <c r="L74" s="69" t="str">
         <f ca="1">IF(K74&lt;=C74, IF(K74&lt;H74,$A$2,IF(K74&lt;H75,$A$3, IF(K74&lt;H76,$A$4, IF(K74&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -9733,7 +10002,7 @@
       <c r="J75" s="69"/>
       <c r="K75" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>29.377597877144701</v>
+        <v>46.556298352208067</v>
       </c>
       <c r="L75" s="69" t="str">
         <f ca="1">IF(K75&lt;=C75, IF(K75&lt;H74,$A$2,IF(K75&lt;H75,$A$3, IF(K75&lt;H76,$A$4, IF(K75&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -9785,7 +10054,7 @@
       <c r="J76" s="69"/>
       <c r="K76" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>46.643831070015551</v>
+        <v>82.692536834696881</v>
       </c>
       <c r="L76" s="69" t="str">
         <f ca="1">IF(K76&lt;=C76, IF(K76&lt;H74,$A$2,IF(K76&lt;H75,$A$3, IF(K76&lt;H76,$A$4, IF(K76&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -9837,7 +10106,7 @@
       <c r="J77" s="69"/>
       <c r="K77" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>18.150841113626704</v>
+        <v>84.428701010115901</v>
       </c>
       <c r="L77" s="69" t="str">
         <f ca="1">IF(K77&lt;=C77, IF(K77&lt;H74,$A$2,IF(K77&lt;H75,$A$3, IF(K77&lt;H76,$A$4, IF(K77&lt;H77,$A$5, "NONE")))), "NONE")</f>
@@ -9887,7 +10156,7 @@
       </c>
       <c r="K78" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>63.839816915964946</v>
+        <v>11.407196706287348</v>
       </c>
       <c r="L78" s="69" t="str">
         <f ca="1">IF(K78&lt;=C78, IF(K78&lt;H78,$A$2,IF(K78&lt;H79,$A$3, IF(K78&lt;H80,$A$4, IF(K78&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -9929,7 +10198,7 @@
       </c>
       <c r="K79" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>55.769659402031166</v>
+        <v>27.928962050825589</v>
       </c>
       <c r="L79" s="69" t="str">
         <f ca="1">IF(K79&lt;=C79, IF(K79&lt;H78,$A$2,IF(K79&lt;H79,$A$3, IF(K79&lt;H80,$A$4, IF(K79&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -9971,7 +10240,7 @@
       </c>
       <c r="K80" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>31.074024460117865</v>
+        <v>95.468266785013569</v>
       </c>
       <c r="L80" s="69" t="str">
         <f ca="1">IF(K80&lt;=C80, IF(K80&lt;H78,$A$2,IF(K80&lt;H79,$A$3, IF(K80&lt;H80,$A$4, IF(K80&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -10013,7 +10282,7 @@
       </c>
       <c r="K81" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>44.115444240277313</v>
+        <v>32.023088176809942</v>
       </c>
       <c r="L81" s="69" t="str">
         <f ca="1">IF(K81&lt;=C81, IF(K81&lt;H78,$A$2,IF(K81&lt;H79,$A$3, IF(K81&lt;H80,$A$4, IF(K81&lt;H81,$A$5, "NONE")))), "NONE")</f>
@@ -10057,7 +10326,7 @@
       <c r="J82" s="69"/>
       <c r="K82" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>45.278241245402597</v>
+        <v>66.761370661701321</v>
       </c>
       <c r="L82" s="69" t="str">
         <f ca="1">IF(K82&lt;=C82, IF(K82&lt;H82,$A$2,IF(K82&lt;H83,$A$3, IF(K82&lt;H84,$A$4, IF(K82&lt;H85,$A$5, "NONE")))), "NONE")</f>
@@ -10109,11 +10378,11 @@
       <c r="J83" s="69"/>
       <c r="K83" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>16.17093937465912</v>
+        <v>10.929806941862374</v>
       </c>
       <c r="L83" s="69" t="str">
         <f ca="1">IF(K83&lt;=C83, IF(K83&lt;H82,$A$2,IF(K83&lt;H83,$A$3, IF(K83&lt;H84,$A$4, IF(K83&lt;H85,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
       <c r="M83" s="69"/>
       <c r="N83" s="69"/>
@@ -10161,7 +10430,7 @@
       <c r="J84" s="69"/>
       <c r="K84" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>60.019269308637014</v>
+        <v>89.405236490417451</v>
       </c>
       <c r="L84" s="69" t="str">
         <f ca="1">IF(K84&lt;=C84, IF(K84&lt;H82,$A$2,IF(K84&lt;H83,$A$3, IF(K84&lt;H84,$A$4, IF(K84&lt;H85,$A$5, "NONE")))), "NONE")</f>
@@ -10213,11 +10482,11 @@
       <c r="J85" s="69"/>
       <c r="K85" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>16.170041880821774</v>
+        <v>9.0596667423590738</v>
       </c>
       <c r="L85" s="69" t="str">
         <f ca="1">IF(K85&lt;=C85, IF(K85&lt;H82,$A$2,IF(K85&lt;H83,$A$3, IF(K85&lt;H84,$A$4, IF(K85&lt;H85,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
       <c r="M85" s="69"/>
       <c r="N85" s="69"/>
@@ -10263,7 +10532,7 @@
       </c>
       <c r="K86" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>60.17151441415136</v>
+        <v>93.092947084601008</v>
       </c>
       <c r="L86" s="69" t="str">
         <f ca="1">IF(K86&lt;=C86, IF(K86&lt;H86,$A$2,IF(K86&lt;H87,$A$3, IF(K86&lt;H88,$A$4, IF(K86&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10305,7 +10574,7 @@
       </c>
       <c r="K87" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>47.873230262778357</v>
+        <v>92.767103091308769</v>
       </c>
       <c r="L87" s="69" t="str">
         <f ca="1">IF(K87&lt;=C87, IF(K87&lt;H86,$A$2,IF(K87&lt;H87,$A$3, IF(K87&lt;H88,$A$4, IF(K87&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10347,7 +10616,7 @@
       </c>
       <c r="K88" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>81.399192718694238</v>
+        <v>25.559181548418188</v>
       </c>
       <c r="L88" s="69" t="str">
         <f ca="1">IF(K88&lt;=C88, IF(K88&lt;H86,$A$2,IF(K88&lt;H87,$A$3, IF(K88&lt;H88,$A$4, IF(K88&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10389,7 +10658,7 @@
       </c>
       <c r="K89" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>80.115614913533818</v>
+        <v>99.883158033421537</v>
       </c>
       <c r="L89" s="69" t="str">
         <f ca="1">IF(K89&lt;=C89, IF(K89&lt;H86,$A$2,IF(K89&lt;H87,$A$3, IF(K89&lt;H88,$A$4, IF(K89&lt;H89,$A$5, "NONE")))), "NONE")</f>
@@ -10433,7 +10702,7 @@
       <c r="J90" s="69"/>
       <c r="K90" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>36.718827630201375</v>
+        <v>25.887764117652711</v>
       </c>
       <c r="L90" s="69" t="str">
         <f ca="1">IF(K90&lt;=C90, IF(K90&lt;H90,$A$2,IF(K90&lt;H91,$A$3, IF(K90&lt;H92,$A$4, IF(K90&lt;H93,$A$5, "NONE")))), "NONE")</f>
@@ -10485,7 +10754,7 @@
       <c r="J91" s="69"/>
       <c r="K91" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>18.055783625014911</v>
+        <v>36.044530971791964</v>
       </c>
       <c r="L91" s="69" t="str">
         <f ca="1">IF(K91&lt;=C91, IF(K91&lt;H90,$A$2,IF(K91&lt;H91,$A$3, IF(K91&lt;H92,$A$4, IF(K91&lt;H93,$A$5, "NONE")))), "NONE")</f>
@@ -10537,7 +10806,7 @@
       <c r="J92" s="69"/>
       <c r="K92" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>30.682266112821555</v>
+        <v>40.186087317194264</v>
       </c>
       <c r="L92" s="69" t="str">
         <f ca="1">IF(K92&lt;=C92, IF(K92&lt;H90,$A$2,IF(K92&lt;H91,$A$3, IF(K92&lt;H92,$A$4, IF(K92&lt;H93,$A$5, "NONE")))), "NONE")</f>
@@ -10589,7 +10858,7 @@
       <c r="J93" s="69"/>
       <c r="K93" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>67.435938371875764</v>
+        <v>51.935045672968549</v>
       </c>
       <c r="L93" s="69" t="str">
         <f ca="1">IF(K93&lt;=C93, IF(K93&lt;H90,$A$2,IF(K93&lt;H91,$A$3, IF(K93&lt;H92,$A$4, IF(K93&lt;H93,$A$5, "NONE")))), "NONE")</f>
@@ -10639,7 +10908,7 @@
       </c>
       <c r="K94" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>13.294382474119459</v>
+        <v>78.680755454656591</v>
       </c>
       <c r="L94" s="69" t="str">
         <f ca="1">IF(K94&lt;=C94, IF(K94&lt;H94,$A$2,IF(K94&lt;H95,$A$3, IF(K94&lt;H96,$A$4, IF(K94&lt;H97,$A$5, "NONE")))), "NONE")</f>
@@ -10681,11 +10950,11 @@
       </c>
       <c r="K95" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>35.789784342126119</v>
+        <v>1.676973717399588</v>
       </c>
       <c r="L95" s="69" t="str">
         <f ca="1">IF(K95&lt;=C95, IF(K95&lt;H94,$A$2,IF(K95&lt;H95,$A$3, IF(K95&lt;H96,$A$4, IF(K95&lt;H97,$A$5, "NONE")))), "NONE")</f>
-        <v>NONE</v>
+        <v>RP_RARE</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
@@ -10723,11 +10992,11 @@
       </c>
       <c r="K96" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>6.3810703944233271</v>
+        <v>32.858685279103625</v>
       </c>
       <c r="L96" s="69" t="str">
         <f ca="1">IF(K96&lt;=C96, IF(K96&lt;H94,$A$2,IF(K96&lt;H95,$A$3, IF(K96&lt;H96,$A$4, IF(K96&lt;H97,$A$5, "NONE")))), "NONE")</f>
-        <v>RP_RARE</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
@@ -10765,7 +11034,7 @@
       </c>
       <c r="K97" s="70">
         <f t="shared" ca="1" si="2"/>
-        <v>70.171163297925034</v>
+        <v>99.973235275577181</v>
       </c>
       <c r="L97" s="69" t="str">
         <f ca="1">IF(K97&lt;=C97, IF(K97&lt;H94,$A$2,IF(K97&lt;H95,$A$3, IF(K97&lt;H96,$A$4, IF(K97&lt;H97,$A$5, "NONE")))), "NONE")</f>
@@ -10989,98 +11258,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8AED65-3B54-4C64-A71C-C47C063CF2F2}">
-  <dimension ref="A2:R22"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="80"/>
-    <col min="2" max="2" width="13.7109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="80" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="82" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="80" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="80" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="80" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="80" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="9" style="80" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="80" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="80" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.42578125" style="80" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="80" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8" style="80" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="80" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" style="80" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="81" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="80"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
+    <row r="1" spans="1:18" s="82" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84" t="s">
+        <v>656</v>
+      </c>
+      <c r="F1" s="84" t="s">
+        <v>657</v>
+      </c>
+      <c r="G1" s="84" t="s">
+        <v>658</v>
+      </c>
+      <c r="H1" s="84" t="s">
+        <v>659</v>
+      </c>
+      <c r="I1" s="84" t="s">
+        <v>660</v>
+      </c>
+      <c r="J1" s="83" t="s">
+        <v>661</v>
+      </c>
+      <c r="K1" s="83" t="s">
+        <v>662</v>
+      </c>
+      <c r="L1" s="84" t="s">
+        <v>663</v>
+      </c>
+      <c r="M1" s="83" t="s">
+        <v>664</v>
+      </c>
+      <c r="N1" s="83" t="s">
+        <v>665</v>
+      </c>
+      <c r="O1" s="84" t="s">
+        <v>666</v>
+      </c>
+      <c r="P1" s="84" t="s">
+        <v>775</v>
+      </c>
+      <c r="Q1" s="83" t="s">
+        <v>667</v>
+      </c>
+      <c r="R1" s="83" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
+        <v>773</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>810</v>
+      </c>
       <c r="D2" s="81" t="s">
-        <v>656</v>
-      </c>
-      <c r="E2" s="81" t="s">
-        <v>657</v>
-      </c>
-      <c r="F2" s="81" t="s">
-        <v>658</v>
-      </c>
-      <c r="G2" s="81" t="s">
-        <v>659</v>
-      </c>
-      <c r="H2" s="81" t="s">
-        <v>660</v>
-      </c>
-      <c r="I2" s="81" t="s">
-        <v>661</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
       <c r="J2" s="81" t="s">
-        <v>662</v>
-      </c>
-      <c r="K2" s="81" t="s">
-        <v>663</v>
-      </c>
-      <c r="L2" s="81" t="s">
-        <v>664</v>
-      </c>
-      <c r="M2" s="81" t="s">
-        <v>665</v>
-      </c>
-      <c r="N2" s="81" t="s">
-        <v>666</v>
-      </c>
-      <c r="O2" s="81" t="s">
-        <v>667</v>
-      </c>
-      <c r="P2" s="81" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q2" s="81" t="s">
-        <v>669</v>
-      </c>
-      <c r="R2" s="80" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
+        <v>772</v>
+      </c>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="80" t="s">
-        <v>745</v>
-      </c>
-      <c r="B3" s="81" t="s">
-        <v>670</v>
+        <v>813</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>671</v>
+        <v>784</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>747</v>
-      </c>
-      <c r="E3" s="81" t="s">
-        <v>748</v>
-      </c>
+        <v>785</v>
+      </c>
+      <c r="E3" s="81"/>
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
       <c r="H3" s="81"/>
@@ -11088,31 +11381,36 @@
       <c r="J3" s="81"/>
       <c r="K3" s="81"/>
       <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
+      <c r="M3" s="81" t="s">
+        <v>772</v>
+      </c>
       <c r="N3" s="81"/>
       <c r="O3" s="81"/>
       <c r="P3" s="81"/>
       <c r="Q3" s="81"/>
     </row>
-    <row r="4" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="81" t="s">
-        <v>674</v>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
+        <v>814</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C4" s="81" t="s">
-        <v>675</v>
+        <v>808</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>747</v>
+        <v>811</v>
       </c>
       <c r="E4" s="81"/>
-      <c r="F4" s="81" t="s">
-        <v>749</v>
-      </c>
+      <c r="F4" s="81"/>
       <c r="G4" s="81"/>
       <c r="H4" s="81"/>
       <c r="I4" s="81"/>
       <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
+      <c r="K4" s="81" t="s">
+        <v>786</v>
+      </c>
       <c r="L4" s="81"/>
       <c r="M4" s="81"/>
       <c r="N4" s="81"/>
@@ -11120,20 +11418,21 @@
       <c r="P4" s="81"/>
       <c r="Q4" s="81"/>
     </row>
-    <row r="5" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="81" t="s">
-        <v>677</v>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="80" t="s">
+        <v>815</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>678</v>
-      </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81" t="s">
-        <v>673</v>
-      </c>
-      <c r="F5" s="81" t="s">
-        <v>676</v>
-      </c>
+        <v>782</v>
+      </c>
+      <c r="D5" s="81" t="s">
+        <v>783</v>
+      </c>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
       <c r="G5" s="81"/>
       <c r="H5" s="81"/>
       <c r="I5" s="81"/>
@@ -11141,22 +11440,29 @@
       <c r="K5" s="81"/>
       <c r="L5" s="81"/>
       <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
+      <c r="N5" s="81" t="s">
+        <v>787</v>
+      </c>
       <c r="O5" s="81"/>
       <c r="P5" s="81"/>
       <c r="Q5" s="81"/>
     </row>
-    <row r="6" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B6" s="81" t="s">
-        <v>679</v>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="80" t="s">
+        <v>816</v>
+      </c>
+      <c r="B6" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>680</v>
+        <v>668</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>756</v>
-      </c>
-      <c r="E6" s="81"/>
+        <v>669</v>
+      </c>
+      <c r="E6" s="81" t="s">
+        <v>788</v>
+      </c>
       <c r="F6" s="81"/>
       <c r="G6" s="81"/>
       <c r="H6" s="81"/>
@@ -11170,18 +11476,23 @@
       <c r="P6" s="81"/>
       <c r="Q6" s="81"/>
     </row>
-    <row r="7" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B7" s="81" t="s">
-        <v>681</v>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="80" t="s">
+        <v>817</v>
+      </c>
+      <c r="B7" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>682</v>
-      </c>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81" t="s">
-        <v>520</v>
-      </c>
-      <c r="F7" s="81"/>
+        <v>670</v>
+      </c>
+      <c r="D7" s="81" t="s">
+        <v>671</v>
+      </c>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81" t="s">
+        <v>788</v>
+      </c>
       <c r="G7" s="81"/>
       <c r="H7" s="81"/>
       <c r="I7" s="81"/>
@@ -11194,19 +11505,24 @@
       <c r="P7" s="81"/>
       <c r="Q7" s="81"/>
     </row>
-    <row r="8" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B8" s="81" t="s">
-        <v>683</v>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="80" t="s">
+        <v>818</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>684</v>
-      </c>
-      <c r="D8" s="81"/>
+        <v>672</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>673</v>
+      </c>
       <c r="E8" s="81"/>
-      <c r="F8" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81" t="s">
+        <v>788</v>
+      </c>
       <c r="H8" s="81"/>
       <c r="I8" s="81"/>
       <c r="J8" s="81"/>
@@ -11218,24 +11534,27 @@
       <c r="P8" s="81"/>
       <c r="Q8" s="81"/>
     </row>
-    <row r="9" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B9" s="81" t="s">
-        <v>685</v>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="80" t="s">
+        <v>819</v>
+      </c>
+      <c r="B9" s="80" t="s">
+        <v>732</v>
       </c>
       <c r="C9" s="81" t="s">
-        <v>686</v>
+        <v>790</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>672</v>
+        <v>789</v>
       </c>
       <c r="E9" s="81"/>
       <c r="F9" s="81"/>
       <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
+      <c r="H9" s="81" t="s">
+        <v>791</v>
+      </c>
       <c r="I9" s="81"/>
-      <c r="J9" s="81" t="s">
-        <v>578</v>
-      </c>
+      <c r="J9" s="81"/>
       <c r="K9" s="81"/>
       <c r="L9" s="81"/>
       <c r="M9" s="81"/>
@@ -11244,229 +11563,646 @@
       <c r="P9" s="81"/>
       <c r="Q9" s="81"/>
     </row>
-    <row r="10" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B10" s="81" t="s">
-        <v>687</v>
-      </c>
-      <c r="C10" s="81" t="s">
-        <v>688</v>
-      </c>
-      <c r="D10" s="81" t="s">
-        <v>672</v>
-      </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81" t="s">
-        <v>575</v>
-      </c>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-    </row>
-    <row r="11" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B11" s="81" t="s">
-        <v>689</v>
-      </c>
-      <c r="C11" s="81" t="s">
-        <v>690</v>
-      </c>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81" t="s">
-        <v>673</v>
-      </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81" t="s">
-        <v>575</v>
-      </c>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-    </row>
-    <row r="12" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B12" s="81" t="s">
-        <v>691</v>
-      </c>
-      <c r="C12" s="81" t="s">
-        <v>692</v>
-      </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81" t="s">
-        <v>673</v>
-      </c>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81" t="s">
-        <v>578</v>
-      </c>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-    </row>
-    <row r="13" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="81" t="s">
-        <v>693</v>
-      </c>
-      <c r="C13" s="81" t="s">
-        <v>694</v>
-      </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81" t="s">
+    <row r="10" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="85" t="s">
+        <v>820</v>
+      </c>
+      <c r="B10" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C10" s="86" t="s">
+        <v>674</v>
+      </c>
+      <c r="D10" s="86" t="s">
+        <v>675</v>
+      </c>
+      <c r="E10" s="86" t="s">
+        <v>774</v>
+      </c>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86" t="s">
+        <v>792</v>
+      </c>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="86"/>
+    </row>
+    <row r="11" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="80" t="s">
+        <v>821</v>
+      </c>
+      <c r="B11" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C11" s="86" t="s">
         <v>676</v>
       </c>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81" t="s">
-        <v>599</v>
-      </c>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-    </row>
-    <row r="14" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B14" s="81" t="s">
-        <v>695</v>
-      </c>
-      <c r="C14" s="81" t="s">
-        <v>696</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81" t="s">
-        <v>676</v>
-      </c>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="81"/>
-    </row>
-    <row r="15" spans="1:18" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="B15" s="81" t="s">
-        <v>697</v>
-      </c>
-      <c r="C15" s="81" t="s">
-        <v>698</v>
-      </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81" t="s">
-        <v>699</v>
-      </c>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="86" t="s">
+        <v>677</v>
+      </c>
+      <c r="E11" s="86" t="s">
+        <v>774</v>
+      </c>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86" t="s">
+        <v>771</v>
+      </c>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+    </row>
+    <row r="12" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="80" t="s">
+        <v>822</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C12" s="86" t="s">
+        <v>678</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>679</v>
+      </c>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86" t="s">
+        <v>774</v>
+      </c>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86" t="s">
+        <v>771</v>
+      </c>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+    </row>
+    <row r="13" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="80" t="s">
+        <v>823</v>
+      </c>
+      <c r="B13" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>680</v>
+      </c>
+      <c r="D13" s="86" t="s">
+        <v>793</v>
+      </c>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86" t="s">
+        <v>774</v>
+      </c>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86" t="s">
+        <v>792</v>
+      </c>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
+    </row>
+    <row r="14" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="80" t="s">
+        <v>824</v>
+      </c>
+      <c r="B14" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C14" s="86" t="s">
+        <v>681</v>
+      </c>
+      <c r="D14" s="86" t="s">
+        <v>682</v>
+      </c>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86" t="s">
+        <v>774</v>
+      </c>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86" t="s">
+        <v>794</v>
+      </c>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="86"/>
+    </row>
+    <row r="15" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="80" t="s">
+        <v>825</v>
+      </c>
+      <c r="B15" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C15" s="86" t="s">
+        <v>683</v>
+      </c>
+      <c r="D15" s="86" t="s">
+        <v>684</v>
+      </c>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86" t="s">
+        <v>774</v>
+      </c>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="86" t="s">
+        <v>769</v>
+      </c>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="86"/>
+    </row>
+    <row r="16" spans="1:18" s="85" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="80" t="s">
+        <v>826</v>
+      </c>
+      <c r="B16" s="85" t="s">
+        <v>732</v>
+      </c>
+      <c r="C16" s="86" t="s">
+        <v>685</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>686</v>
+      </c>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86" t="s">
+        <v>795</v>
+      </c>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="86" t="s">
+        <v>771</v>
+      </c>
+      <c r="R16" s="86"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
+        <v>827</v>
+      </c>
+      <c r="B17" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C17" s="81" t="s">
+        <v>797</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>796</v>
+      </c>
+      <c r="E17" s="81"/>
+      <c r="F17" s="81"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="81" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="80" t="s">
+        <v>828</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>799</v>
+      </c>
+      <c r="D18" s="81" t="s">
+        <v>798</v>
+      </c>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+      <c r="P18" s="81"/>
+      <c r="Q18" s="81" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="80" t="s">
+        <v>829</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>801</v>
+      </c>
+      <c r="D19" s="81" t="s">
+        <v>800</v>
+      </c>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="81"/>
+      <c r="P19" s="81" t="s">
+        <v>786</v>
+      </c>
+      <c r="Q19" s="81"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="80" t="s">
+        <v>830</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C20" s="81" t="s">
+        <v>803</v>
+      </c>
+      <c r="D20" s="81" t="s">
+        <v>802</v>
+      </c>
+      <c r="E20" s="81"/>
+      <c r="F20" s="81"/>
+      <c r="G20" s="81"/>
+      <c r="H20" s="81"/>
+      <c r="I20" s="81"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="81"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="81" t="s">
+        <v>804</v>
+      </c>
+      <c r="P20" s="81"/>
+      <c r="Q20" s="81"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="80" t="s">
+        <v>831</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>732</v>
+      </c>
+      <c r="C21" s="81" t="s">
+        <v>806</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>805</v>
+      </c>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81" t="s">
+        <v>807</v>
+      </c>
+      <c r="M21" s="81"/>
+      <c r="N21" s="81"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="81"/>
+      <c r="Q21" s="81"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="80" t="s">
+        <v>832</v>
+      </c>
+      <c r="B22" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C22" s="80" t="s">
+        <v>735</v>
+      </c>
+      <c r="D22" s="80" t="s">
+        <v>734</v>
+      </c>
+      <c r="E22" s="80" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="80" t="s">
+        <v>833</v>
+      </c>
+      <c r="B23" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C23" s="80" t="s">
+        <v>738</v>
+      </c>
+      <c r="D23" s="80" t="s">
+        <v>737</v>
+      </c>
+      <c r="E23" s="80" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="80" t="s">
+        <v>834</v>
+      </c>
+      <c r="B24" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C24" s="80" t="s">
+        <v>747</v>
+      </c>
+      <c r="D24" s="80" t="s">
+        <v>740</v>
+      </c>
+      <c r="F24" s="80" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="80" t="s">
+        <v>835</v>
+      </c>
+      <c r="B25" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C25" s="80" t="s">
+        <v>742</v>
+      </c>
+      <c r="D25" s="80" t="s">
+        <v>741</v>
+      </c>
+      <c r="F25" s="80" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="80" t="s">
+        <v>836</v>
+      </c>
+      <c r="B26" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C26" s="80" t="s">
+        <v>744</v>
+      </c>
+      <c r="D26" s="80" t="s">
+        <v>743</v>
+      </c>
+      <c r="G26" s="80" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="80" t="s">
+        <v>837</v>
+      </c>
+      <c r="B27" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C27" s="80" t="s">
         <v>746</v>
       </c>
-      <c r="B17" s="80" t="s">
+      <c r="D27" s="80" t="s">
+        <v>745</v>
+      </c>
+      <c r="G27" s="80" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="80" t="s">
+        <v>838</v>
+      </c>
+      <c r="B28" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C28" s="80" t="s">
         <v>751</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="D28" s="80" t="s">
+        <v>748</v>
+      </c>
+      <c r="H28" s="80" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="80" t="s">
+        <v>839</v>
+      </c>
+      <c r="B29" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C29" s="80" t="s">
         <v>750</v>
       </c>
-      <c r="D17" s="82" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="80" t="s">
+      <c r="D29" s="80" t="s">
+        <v>749</v>
+      </c>
+      <c r="H29" s="80" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="80" t="s">
+        <v>840</v>
+      </c>
+      <c r="B30" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C30" s="80" t="s">
         <v>754</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="D30" s="80" t="s">
         <v>753</v>
       </c>
-      <c r="D18" s="82" t="s">
+      <c r="I30" s="80" t="s">
         <v>755</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="80" t="s">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="80" t="s">
+        <v>841</v>
+      </c>
+      <c r="B31" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C31" s="80" t="s">
+        <v>766</v>
+      </c>
+      <c r="D31" s="80" t="s">
+        <v>812</v>
+      </c>
+      <c r="I31" s="80" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="80" t="s">
+        <v>842</v>
+      </c>
+      <c r="B32" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C32" s="80" t="s">
+        <v>757</v>
+      </c>
+      <c r="D32" s="80" t="s">
+        <v>756</v>
+      </c>
+      <c r="L32" s="80" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="80" t="s">
+        <v>843</v>
+      </c>
+      <c r="B33" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>759</v>
+      </c>
+      <c r="D33" s="80" t="s">
         <v>758</v>
       </c>
-      <c r="C19" s="80" t="s">
-        <v>757</v>
-      </c>
-      <c r="E19" s="82" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="80" t="s">
-        <v>760</v>
-      </c>
-      <c r="C20" s="80" t="s">
-        <v>759</v>
-      </c>
-      <c r="E20" s="82" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="80" t="s">
-        <v>762</v>
-      </c>
-      <c r="C21" s="80" t="s">
-        <v>761</v>
-      </c>
-      <c r="F21" s="82" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="80" t="s">
+      <c r="L33" s="80" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="80" t="s">
+        <v>844</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C34" s="80" t="s">
+        <v>765</v>
+      </c>
+      <c r="D34" s="80" t="s">
         <v>764</v>
       </c>
-      <c r="C22" s="80" t="s">
-        <v>763</v>
-      </c>
-      <c r="F22" s="82" t="s">
-        <v>755</v>
+      <c r="O34" s="80" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="80" t="s">
+        <v>845</v>
+      </c>
+      <c r="B35" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C35" s="80" t="s">
+        <v>768</v>
+      </c>
+      <c r="D35" s="80" t="s">
+        <v>767</v>
+      </c>
+      <c r="O35" s="80" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="80" t="s">
+        <v>846</v>
+      </c>
+      <c r="B36" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C36" s="80" t="s">
+        <v>777</v>
+      </c>
+      <c r="D36" s="80" t="s">
+        <v>776</v>
+      </c>
+      <c r="P36" s="80" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="80" t="s">
+        <v>847</v>
+      </c>
+      <c r="B37" s="80" t="s">
+        <v>733</v>
+      </c>
+      <c r="C37" s="80" t="s">
+        <v>779</v>
+      </c>
+      <c r="D37" s="80" t="s">
+        <v>778</v>
+      </c>
+      <c r="P37" s="80" t="s">
+        <v>781</v>
       </c>
     </row>
   </sheetData>
@@ -11477,10 +12213,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B7EA3C-4ADA-4CF3-81F5-CEFF874C559A}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11491,11 +12228,11 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11512,18 +12249,18 @@
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="10" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="16"/>
       <c r="C5" s="18" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11533,45 +12270,45 @@
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="10" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="10" t="s">
-        <v>709</v>
+        <v>696</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="10" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="65" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="65"/>
       <c r="B12" s="13"/>
       <c r="C12" s="10" t="s">
-        <v>713</v>
+        <v>700</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11581,18 +12318,18 @@
     </row>
     <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="65" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="65"/>
       <c r="B15" s="13"/>
       <c r="C15" s="10" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11602,11 +12339,11 @@
     </row>
     <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="65" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11618,18 +12355,18 @@
     </row>
     <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="15"/>
       <c r="C21" s="10" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11639,11 +12376,11 @@
     </row>
     <row r="23" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11660,34 +12397,34 @@
     </row>
     <row r="26" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>720</v>
+        <v>707</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="10" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A27" s="10"/>
       <c r="B27" s="15"/>
       <c r="C27" s="10" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="53" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="3"/>
       <c r="C30" s="53" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11697,11 +12434,11 @@
     </row>
     <row r="32" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="53" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11718,11 +12455,11 @@
     </row>
     <row r="35" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="53" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11733,29 +12470,29 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="77" t="s">
-        <v>725</v>
+      <c r="A38" s="76" t="s">
+        <v>712</v>
       </c>
       <c r="B38" s="16"/>
       <c r="C38" s="10" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="77"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="16"/>
       <c r="C39" s="17" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="77"/>
+      <c r="A40" s="76"/>
       <c r="B40" s="16"/>
       <c r="C40" s="10"/>
     </row>
     <row r="41" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="77" t="s">
-        <v>728</v>
+      <c r="A41" s="76" t="s">
+        <v>715</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="10" t="s">
@@ -11763,26 +12500,26 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="77"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="16"/>
       <c r="C42" s="17" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="78" t="s">
-        <v>730</v>
+      <c r="A44" s="77" t="s">
+        <v>717</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="17" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A45" s="65"/>
       <c r="B45" s="14"/>
       <c r="C45" s="18" t="s">
-        <v>732</v>
+        <v>719</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11791,7 +12528,7 @@
       <c r="C46" s="10"/>
     </row>
     <row r="47" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="78" t="s">
+      <c r="A47" s="77" t="s">
         <v>88</v>
       </c>
       <c r="B47" s="14"/>
@@ -11814,26 +12551,26 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="77" t="s">
-        <v>733</v>
+      <c r="A51" s="76" t="s">
+        <v>720</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="10" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>
       <c r="B52" s="16"/>
       <c r="C52" s="17" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A53" s="10"/>
       <c r="B53" s="16"/>
       <c r="C53" s="18" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
@@ -11842,8 +12579,8 @@
       <c r="C54" s="10"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="77" t="s">
-        <v>737</v>
+      <c r="A55" s="76" t="s">
+        <v>724</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="10" t="s">
@@ -11854,32 +12591,32 @@
       <c r="A56" s="10"/>
       <c r="B56" s="15"/>
       <c r="C56" s="10" t="s">
-        <v>738</v>
+        <v>725</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="79" t="s">
-        <v>739</v>
+      <c r="A58" s="78" t="s">
+        <v>726</v>
       </c>
       <c r="B58" s="61" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
       <c r="C58" s="53" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A59" s="11"/>
       <c r="B59" s="61"/>
       <c r="C59" s="58" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A60" s="11"/>
       <c r="B60" s="61"/>
       <c r="C60" s="55" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
     </row>
   </sheetData>
@@ -11892,8 +12629,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -13775,8 +14512,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -14627,7 +15364,7 @@
   <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -15094,7 +15831,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -16981,18 +17718,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="79" t="s">
         <v>626</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="71"/>

</xml_diff>